<commit_message>
updated fluorometer CC_scattering_angle and CC_angular_resolution
Updated fluorometer calibration coefficients according to the following:

FLORT D, J, K, M, N, O
FLORD D:

CC_scattering_angle = 124
CC_angular_resolution = 1.076

FLORD G, L, M
FLNTU A:

CC_scattering_angle = 140
CC_angular_resolution = 1.096
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE04OSPD.xlsx
+++ b/deployment/Omaha_Cal_Info_CE04OSPD.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="9680" yWindow="940" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Moorings" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Asset_Cal_Info" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="IntegrationEvents" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Verification" sheetId="4" r:id="rId6"/>
+    <sheet name="Moorings" sheetId="1" r:id="rId1"/>
+    <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
+    <sheet name="IntegrationEvents" sheetId="3" r:id="rId3"/>
+    <sheet name="Verification" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -19,47 +27,96 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E3">
+    <comment ref="E3" authorId="0">
       <text>
-        <t xml:space="preserve">equipment list as ATAPL-58320, but that is too short
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>equipment list as ATAPL-58320, but that is too short
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F3">
+    <comment ref="F3" authorId="0">
       <text>
-        <t xml:space="preserve">equipment list shows 137
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>equipment list shows 137
 bulk load has 215
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E50">
+    <comment ref="E20" authorId="0">
       <text>
-        <t xml:space="preserve">missing from bulk load
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>missing from bulk load
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E41">
+    <comment ref="E32" authorId="0">
       <text>
-        <t xml:space="preserve">missing from bulk load
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>missing from bulk load
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E32">
+    <comment ref="H32" authorId="0">
       <text>
-        <t xml:space="preserve">missing from bulk load
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>not sure if these calibration values were for the first or second deployment - just duplicated them - applies to all instruments
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="H32">
+    <comment ref="E41" authorId="0">
       <text>
-        <t xml:space="preserve">not sure if these calibration values were for the first or second deployment - just duplicated them - applies to all instruments
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>missing from bulk load
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E20">
+    <comment ref="E50" authorId="0">
       <text>
-        <t xml:space="preserve">missing from bulk load
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>missing from bulk load
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -72,10 +129,17 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C2">
+    <comment ref="C2" authorId="0">
       <text>
-        <t xml:space="preserve">no data, so it doesn't show up in the UI with a name :(
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>no data, so it doesn't show up in the UI with a name :(
 	-Dan Mergens</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -351,44 +415,48 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="166" formatCode="m&quot;/&quot;d&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF999999"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -397,7 +465,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -430,6 +498,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -442,6 +511,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -452,264 +522,665 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="74">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="15" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1031" name="Rectangle 7" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.29"/>
-    <col customWidth="1" min="2" max="2" width="33.14"/>
-    <col customWidth="1" min="3" max="3" width="24.57"/>
-    <col customWidth="1" min="4" max="7" width="12.0"/>
-    <col customWidth="1" min="8" max="11" width="14.43"/>
-    <col customWidth="1" min="12" max="12" width="18.14"/>
-    <col customWidth="1" min="13" max="14" width="14.43"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="7" width="12" customWidth="1"/>
+    <col min="8" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
+    <col min="13" max="14" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.0" customHeight="1">
+    <row r="1" spans="1:14" ht="27" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +1220,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -760,13 +1231,13 @@
         <v>14</v>
       </c>
       <c r="D2" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="7">
-        <v>41867.0</v>
+        <v>41867</v>
       </c>
       <c r="F2" s="8">
-        <v>0.9791666666666666</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="10" t="s">
@@ -776,7 +1247,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="11">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>17</v>
@@ -784,16 +1255,16 @@
       <c r="L2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="13" t="str">
-        <f t="shared" ref="M2:M7" si="1">((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
-        <v>44.36831</v>
-      </c>
-      <c r="N2" s="13" t="str">
-        <f t="shared" ref="N2:N7" si="2">((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
+      <c r="M2" s="13">
+        <f t="shared" ref="M2:M7" si="0">((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
+        <v>44.368310000000001</v>
+      </c>
+      <c r="N2" s="13">
+        <f t="shared" ref="N2:N7" si="1">((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
@@ -804,13 +1275,13 @@
         <v>21</v>
       </c>
       <c r="D3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="7">
-        <v>41867.0</v>
+        <v>41867</v>
       </c>
       <c r="F3" s="8">
-        <v>0.9791666666666666</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="17" t="s">
@@ -820,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="11">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>17</v>
@@ -828,16 +1299,16 @@
       <c r="L3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="13" t="str">
+      <c r="M3" s="13">
+        <f t="shared" si="0"/>
+        <v>44.368310000000001</v>
+      </c>
+      <c r="N3" s="13">
         <f t="shared" si="1"/>
-        <v>44.36831</v>
-      </c>
-      <c r="N3" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>22</v>
       </c>
@@ -845,16 +1316,16 @@
         <v>23</v>
       </c>
       <c r="C4" s="16">
-        <v>1131.0</v>
+        <v>1131</v>
       </c>
       <c r="D4" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="7">
-        <v>41867.0</v>
+        <v>41867</v>
       </c>
       <c r="F4" s="8">
-        <v>0.9791666666666666</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="17" t="s">
@@ -864,7 +1335,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="11">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>17</v>
@@ -872,16 +1343,16 @@
       <c r="L4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="13" t="str">
+      <c r="M4" s="13">
+        <f t="shared" si="0"/>
+        <v>44.368310000000001</v>
+      </c>
+      <c r="N4" s="13">
         <f t="shared" si="1"/>
-        <v>44.36831</v>
-      </c>
-      <c r="N4" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -889,16 +1360,16 @@
         <v>25</v>
       </c>
       <c r="C5" s="16">
-        <v>3400.0</v>
+        <v>3400</v>
       </c>
       <c r="D5" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="7">
-        <v>41867.0</v>
+        <v>41867</v>
       </c>
       <c r="F5" s="8">
-        <v>0.9791666666666666</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="17" t="s">
@@ -908,7 +1379,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="11">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>17</v>
@@ -916,16 +1387,16 @@
       <c r="L5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="13" t="str">
+      <c r="M5" s="13">
+        <f t="shared" si="0"/>
+        <v>44.368310000000001</v>
+      </c>
+      <c r="N5" s="13">
         <f t="shared" si="1"/>
-        <v>44.36831</v>
-      </c>
-      <c r="N5" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -933,16 +1404,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="16">
-        <v>3398.0</v>
+        <v>3398</v>
       </c>
       <c r="D6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="7">
-        <v>41867.0</v>
+        <v>41867</v>
       </c>
       <c r="F6" s="8">
-        <v>0.9791666666666666</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="17" t="s">
@@ -952,7 +1423,7 @@
         <v>16</v>
       </c>
       <c r="J6" s="11">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>17</v>
@@ -960,16 +1431,16 @@
       <c r="L6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="13" t="str">
+      <c r="M6" s="13">
+        <f t="shared" si="0"/>
+        <v>44.368310000000001</v>
+      </c>
+      <c r="N6" s="13">
         <f t="shared" si="1"/>
-        <v>44.36831</v>
-      </c>
-      <c r="N6" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -977,16 +1448,16 @@
         <v>29</v>
       </c>
       <c r="C7" s="18">
-        <v>137.0</v>
+        <v>137</v>
       </c>
       <c r="D7" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="7">
-        <v>41867.0</v>
+        <v>41867</v>
       </c>
       <c r="F7" s="8">
-        <v>0.9791666666666666</v>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="10" t="s">
@@ -996,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="11">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>17</v>
@@ -1004,16 +1475,16 @@
       <c r="L7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="13" t="str">
+      <c r="M7" s="13">
+        <f t="shared" si="0"/>
+        <v>44.368310000000001</v>
+      </c>
+      <c r="N7" s="13">
         <f t="shared" si="1"/>
-        <v>44.36831</v>
-      </c>
-      <c r="N7" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="19"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1029,7 +1500,7 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>30</v>
       </c>
@@ -1040,13 +1511,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="9">
-        <v>42209.0</v>
+        <v>42209</v>
       </c>
       <c r="F9" s="8">
-        <v>0.8263888888888888</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="10" t="s">
@@ -1056,7 +1527,7 @@
         <v>32</v>
       </c>
       <c r="J9" s="17">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>33</v>
@@ -1064,16 +1535,16 @@
       <c r="L9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="13" t="str">
-        <f t="shared" ref="M9:M14" si="3">((LEFT(H9,(FIND("°",H9,1)-1)))+(MID(H9,(FIND("°",H9,1)+1),(FIND("'",H9,1))-(FIND("°",H9,1)+1))/60))*(IF(RIGHT(H9,1)="N",1,-1))</f>
-        <v>44.36829167</v>
-      </c>
-      <c r="N9" s="13" t="str">
-        <f t="shared" ref="N9:N14" si="4">((LEFT(I9,(FIND("°",I9,1)-1)))+(MID(I9,(FIND("°",I9,1)+1),(FIND("'",I9,1))-(FIND("°",I9,1)+1))/60))*(IF(RIGHT(I9,1)="E",1,-1))</f>
-        <v>-124.9527967</v>
-      </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
+      <c r="M9" s="13">
+        <f t="shared" ref="M9:M14" si="2">((LEFT(H9,(FIND("°",H9,1)-1)))+(MID(H9,(FIND("°",H9,1)+1),(FIND("'",H9,1))-(FIND("°",H9,1)+1))/60))*(IF(RIGHT(H9,1)="N",1,-1))</f>
+        <v>44.368291666666664</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" ref="N9:N14" si="3">((LEFT(I9,(FIND("°",I9,1)-1)))+(MID(I9,(FIND("°",I9,1)+1),(FIND("'",I9,1))-(FIND("°",I9,1)+1))/60))*(IF(RIGHT(I9,1)="E",1,-1))</f>
+        <v>-124.95279666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="12.75" customHeight="1">
       <c r="A10" s="23" t="s">
         <v>35</v>
       </c>
@@ -1084,13 +1555,13 @@
         <v>36</v>
       </c>
       <c r="D10" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="9">
-        <v>42209.0</v>
+        <v>42209</v>
       </c>
       <c r="F10" s="8">
-        <v>0.8263888888888888</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="17" t="s">
@@ -1100,7 +1571,7 @@
         <v>32</v>
       </c>
       <c r="J10" s="17">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>33</v>
@@ -1108,16 +1579,16 @@
       <c r="L10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="13" t="str">
+      <c r="M10" s="13">
+        <f t="shared" si="2"/>
+        <v>44.368291666666664</v>
+      </c>
+      <c r="N10" s="13">
         <f t="shared" si="3"/>
-        <v>44.36829167</v>
-      </c>
-      <c r="N10" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>-124.9527967</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
+        <v>-124.95279666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="12.75" customHeight="1">
       <c r="A11" s="23" t="s">
         <v>38</v>
       </c>
@@ -1125,16 +1596,16 @@
         <v>23</v>
       </c>
       <c r="C11" s="10">
-        <v>1216.0</v>
+        <v>1216</v>
       </c>
       <c r="D11" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="9">
-        <v>42209.0</v>
+        <v>42209</v>
       </c>
       <c r="F11" s="8">
-        <v>0.8263888888888888</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="17" t="s">
@@ -1144,7 +1615,7 @@
         <v>32</v>
       </c>
       <c r="J11" s="17">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>33</v>
@@ -1152,16 +1623,16 @@
       <c r="L11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="13" t="str">
+      <c r="M11" s="13">
+        <f t="shared" si="2"/>
+        <v>44.368291666666664</v>
+      </c>
+      <c r="N11" s="13">
         <f t="shared" si="3"/>
-        <v>44.36829167</v>
-      </c>
-      <c r="N11" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>-124.9527967</v>
-      </c>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
+        <v>-124.95279666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="12.75" customHeight="1">
       <c r="A12" s="23" t="s">
         <v>39</v>
       </c>
@@ -1169,16 +1640,16 @@
         <v>25</v>
       </c>
       <c r="C12" s="10">
-        <v>3717.0</v>
+        <v>3717</v>
       </c>
       <c r="D12" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="9">
-        <v>42209.0</v>
+        <v>42209</v>
       </c>
       <c r="F12" s="8">
-        <v>0.8263888888888888</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="17" t="s">
@@ -1188,7 +1659,7 @@
         <v>32</v>
       </c>
       <c r="J12" s="17">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>33</v>
@@ -1196,16 +1667,16 @@
       <c r="L12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="13" t="str">
+      <c r="M12" s="13">
+        <f t="shared" si="2"/>
+        <v>44.368291666666664</v>
+      </c>
+      <c r="N12" s="13">
         <f t="shared" si="3"/>
-        <v>44.36829167</v>
-      </c>
-      <c r="N12" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>-124.9527967</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
+        <v>-124.95279666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="12.75" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>40</v>
       </c>
@@ -1213,16 +1684,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="10">
-        <v>3762.0</v>
+        <v>3762</v>
       </c>
       <c r="D13" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="9">
-        <v>42209.0</v>
+        <v>42209</v>
       </c>
       <c r="F13" s="8">
-        <v>0.8263888888888888</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="17" t="s">
@@ -1232,7 +1703,7 @@
         <v>32</v>
       </c>
       <c r="J13" s="17">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>33</v>
@@ -1240,16 +1711,16 @@
       <c r="L13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="13" t="str">
+      <c r="M13" s="13">
+        <f t="shared" si="2"/>
+        <v>44.368291666666664</v>
+      </c>
+      <c r="N13" s="13">
         <f t="shared" si="3"/>
-        <v>44.36829167</v>
-      </c>
-      <c r="N13" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>-124.9527967</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
+        <v>-124.95279666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="12.75" customHeight="1">
       <c r="A14" s="23" t="s">
         <v>42</v>
       </c>
@@ -1257,16 +1728,16 @@
         <v>29</v>
       </c>
       <c r="C14" s="10">
-        <v>317.0</v>
+        <v>317</v>
       </c>
       <c r="D14" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="9">
-        <v>42209.0</v>
+        <v>42209</v>
       </c>
       <c r="F14" s="8">
-        <v>0.8263888888888888</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="10" t="s">
@@ -1276,7 +1747,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="17">
-        <v>582.0</v>
+        <v>582</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>33</v>
@@ -1284,16 +1755,16 @@
       <c r="L14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="M14" s="13" t="str">
+      <c r="M14" s="13">
+        <f t="shared" si="2"/>
+        <v>44.368291666666664</v>
+      </c>
+      <c r="N14" s="13">
         <f t="shared" si="3"/>
-        <v>44.36829167</v>
-      </c>
-      <c r="N14" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>-124.9527967</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
+        <v>-124.95279666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
@@ -1309,7 +1780,7 @@
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
+    <row r="16" spans="1:14" ht="12.75" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
@@ -1325,7 +1796,7 @@
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
+    <row r="17" spans="1:14" ht="12.75" customHeight="1">
       <c r="A17" s="19"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -1341,7 +1812,7 @@
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
     </row>
-    <row r="18" ht="12.75" customHeight="1">
+    <row r="18" spans="1:14" ht="12.75" customHeight="1">
       <c r="A18" s="19"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -1357,7 +1828,7 @@
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1">
+    <row r="19" spans="1:14" ht="12.75" customHeight="1">
       <c r="A19" s="19"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -1373,7 +1844,7 @@
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
+    <row r="20" spans="1:14" ht="12.75" customHeight="1">
       <c r="A20" s="19"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -1390,32 +1861,38 @@
       <c r="N20" s="28"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.86"/>
-    <col customWidth="1" min="2" max="2" width="19.86"/>
-    <col customWidth="1" min="3" max="3" width="23.57"/>
-    <col customWidth="1" min="4" max="4" width="13.14"/>
-    <col customWidth="1" min="5" max="5" width="20.43"/>
-    <col customWidth="1" min="6" max="6" width="14.29"/>
-    <col customWidth="1" min="7" max="7" width="29.86"/>
-    <col customWidth="1" min="8" max="8" width="59.29"/>
-    <col customWidth="1" min="9" max="9" width="15.71"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="59.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1444,81 +1921,81 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="30"/>
       <c r="B2" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!A:A,Moorings!B:B=left(A2,14),Moorings!D:D=D2))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!A:A,Moorings!B:B=left(A2,14),Moorings!D:D=D2))"),"")</f>
         <v/>
       </c>
       <c r="C2" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!C:C,Moorings!B:B=left(A2,14),Moorings!D:D=D2))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!C:C,Moorings!B:B=left(A2,14),Moorings!D:D=D2))"),"")</f>
         <v/>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!A:A,Moorings!B:B=A2,Moorings!D:D=D2))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!A:A,Moorings!B:B=A2,Moorings!D:D=D2))"),"")</f>
         <v/>
       </c>
       <c r="F2" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!C:C,Moorings!B:B=A2,Moorings!D:D=D2))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!C:C,Moorings!B:B=A2,Moorings!D:D=D2))"),"")</f>
         <v/>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="31"/>
       <c r="I2" s="32"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!A:A,Moorings!B:B=left(A3,14),Moorings!D:D=D3))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!A:A,Moorings!B:B=left(A3,14),Moorings!D:D=D3))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C3" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!C:C,Moorings!B:B=left(A3,14),Moorings!D:D=D3))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!C:C,Moorings!B:B=left(A3,14),Moorings!D:D=D3))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D3" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!A:A,Moorings!B:B=A3,Moorings!D:D=D3))"),"A00175")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!A:A,Moorings!B:B=A3,Moorings!D:D=D3))"),"A00175")</f>
         <v>A00175</v>
       </c>
       <c r="F3" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!C:C,Moorings!B:B=A3,Moorings!D:D=D3))"),"137")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A3),"""",filter(Moorings!C:C,Moorings!B:B=A3,Moorings!D:D=D3))"),"137")</f>
         <v>137</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="36">
-        <v>44.3682766666666</v>
+        <v>44.368276666666603</v>
       </c>
       <c r="I3" s="37"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!A:A,Moorings!B:B=left(A4,14),Moorings!D:D=D4))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!A:A,Moorings!B:B=left(A4,14),Moorings!D:D=D4))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C4" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!C:C,Moorings!B:B=left(A4,14),Moorings!D:D=D4))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!C:C,Moorings!B:B=left(A4,14),Moorings!D:D=D4))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D4" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!A:A,Moorings!B:B=A4,Moorings!D:D=D4))"),"A00175")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!A:A,Moorings!B:B=A4,Moorings!D:D=D4))"),"A00175")</f>
         <v>A00175</v>
       </c>
       <c r="F4" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!C:C,Moorings!B:B=A4,Moorings!D:D=D4))"),"137")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A4),"""",filter(Moorings!C:C,Moorings!B:B=A4,Moorings!D:D=D4))"),"137")</f>
         <v>137</v>
       </c>
       <c r="G4" s="35" t="s">
@@ -1529,27 +2006,27 @@
       </c>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!A:A,Moorings!B:B=left(A5,14),Moorings!D:D=D5))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!A:A,Moorings!B:B=left(A5,14),Moorings!D:D=D5))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C5" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!C:C,Moorings!B:B=left(A5,14),Moorings!D:D=D5))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!C:C,Moorings!B:B=left(A5,14),Moorings!D:D=D5))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D5" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!A:A,Moorings!B:B=A5,Moorings!D:D=D5))"),"A00175")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!A:A,Moorings!B:B=A5,Moorings!D:D=D5))"),"A00175")</f>
         <v>A00175</v>
       </c>
       <c r="F5" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!C:C,Moorings!B:B=A5,Moorings!D:D=D5))"),"137")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!C:C,Moorings!B:B=A5,Moorings!D:D=D5))"),"137")</f>
         <v>137</v>
       </c>
       <c r="G5" s="35" t="s">
@@ -1560,81 +2037,81 @@
       </c>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="33"/>
       <c r="B6" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!A:A,Moorings!B:B=left(A6,14),Moorings!D:D=D6))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!A:A,Moorings!B:B=left(A6,14),Moorings!D:D=D6))"),"")</f>
         <v/>
       </c>
       <c r="C6" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!C:C,Moorings!B:B=left(A6,14),Moorings!D:D=D6))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!C:C,Moorings!B:B=left(A6,14),Moorings!D:D=D6))"),"")</f>
         <v/>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!A:A,Moorings!B:B=A6,Moorings!D:D=D6))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!A:A,Moorings!B:B=A6,Moorings!D:D=D6))"),"")</f>
         <v/>
       </c>
       <c r="F6" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!C:C,Moorings!B:B=A6,Moorings!D:D=D6))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!C:C,Moorings!B:B=A6,Moorings!D:D=D6))"),"")</f>
         <v/>
       </c>
       <c r="G6" s="35"/>
       <c r="H6" s="36"/>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1">
       <c r="A7" s="40" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!A:A,Moorings!B:B=left(A7,14),Moorings!D:D=D7))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!A:A,Moorings!B:B=left(A7,14),Moorings!D:D=D7))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C7" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!C:C,Moorings!B:B=left(A7,14),Moorings!D:D=D7))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!C:C,Moorings!B:B=left(A7,14),Moorings!D:D=D7))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D7" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!A:A,Moorings!B:B=A7,Moorings!D:D=D7))"),"ATOSU-58320-00018")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!A:A,Moorings!B:B=A7,Moorings!D:D=D7))"),"ATOSU-58320-00018")</f>
         <v>ATOSU-58320-00018</v>
       </c>
       <c r="F7" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!C:C,Moorings!B:B=A7,Moorings!D:D=D7))"),"317")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A7),"""",filter(Moorings!C:C,Moorings!B:B=A7,Moorings!D:D=D7))"),"317")</f>
         <v>317</v>
       </c>
       <c r="G7" s="42" t="s">
         <v>48</v>
       </c>
       <c r="H7" s="43">
-        <v>44.3682766666666</v>
+        <v>44.368276666666603</v>
       </c>
       <c r="I7" s="44"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1">
       <c r="A8" s="40" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!A:A,Moorings!B:B=left(A8,14),Moorings!D:D=D8))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!A:A,Moorings!B:B=left(A8,14),Moorings!D:D=D8))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C8" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!C:C,Moorings!B:B=left(A8,14),Moorings!D:D=D8))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!C:C,Moorings!B:B=left(A8,14),Moorings!D:D=D8))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D8" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!A:A,Moorings!B:B=A8,Moorings!D:D=D8))"),"ATOSU-58320-00018")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!A:A,Moorings!B:B=A8,Moorings!D:D=D8))"),"ATOSU-58320-00018")</f>
         <v>ATOSU-58320-00018</v>
       </c>
       <c r="F8" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!C:C,Moorings!B:B=A8,Moorings!D:D=D8))"),"317")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!C:C,Moorings!B:B=A8,Moorings!D:D=D8))"),"317")</f>
         <v>317</v>
       </c>
       <c r="G8" s="42" t="s">
@@ -1645,27 +2122,27 @@
       </c>
       <c r="I8" s="44"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="42" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!A:A,Moorings!B:B=left(A9,14),Moorings!D:D=D9))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!A:A,Moorings!B:B=left(A9,14),Moorings!D:D=D9))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C9" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!C:C,Moorings!B:B=left(A9,14),Moorings!D:D=D9))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!C:C,Moorings!B:B=left(A9,14),Moorings!D:D=D9))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D9" s="45">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!A:A,Moorings!B:B=A9,Moorings!D:D=D9))"),"ATOSU-58320-00018")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!A:A,Moorings!B:B=A9,Moorings!D:D=D9))"),"ATOSU-58320-00018")</f>
         <v>ATOSU-58320-00018</v>
       </c>
       <c r="F9" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!C:C,Moorings!B:B=A9,Moorings!D:D=D9))"),"317")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A9),"""",filter(Moorings!C:C,Moorings!B:B=A9,Moorings!D:D=D9))"),"317")</f>
         <v>317</v>
       </c>
       <c r="G9" s="42" t="s">
@@ -1676,762 +2153,762 @@
       </c>
       <c r="I9" s="42"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="47"/>
       <c r="B10" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!A:A,Moorings!B:B=left(A10,14),Moorings!D:D=D10))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!A:A,Moorings!B:B=left(A10,14),Moorings!D:D=D10))"),"")</f>
         <v/>
       </c>
       <c r="C10" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!C:C,Moorings!B:B=left(A10,14),Moorings!D:D=D10))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!C:C,Moorings!B:B=left(A10,14),Moorings!D:D=D10))"),"")</f>
         <v/>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!A:A,Moorings!B:B=A10,Moorings!D:D=D10))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!A:A,Moorings!B:B=A10,Moorings!D:D=D10))"),"")</f>
         <v/>
       </c>
       <c r="F10" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!C:C,Moorings!B:B=A10,Moorings!D:D=D10))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!C:C,Moorings!B:B=A10,Moorings!D:D=D10))"),"")</f>
         <v/>
       </c>
       <c r="G10" s="35"/>
       <c r="H10" s="48"/>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1">
       <c r="A11" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!A:A,Moorings!B:B=left(A11,14),Moorings!D:D=D11))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!A:A,Moorings!B:B=left(A11,14),Moorings!D:D=D11))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C11" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!C:C,Moorings!B:B=left(A11,14),Moorings!D:D=D11))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!C:C,Moorings!B:B=left(A11,14),Moorings!D:D=D11))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D11" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!A:A,Moorings!B:B=A11,Moorings!D:D=D11))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!A:A,Moorings!B:B=A11,Moorings!D:D=D11))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F11" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!C:C,Moorings!B:B=A11,Moorings!D:D=D11))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A11),"""",filter(Moorings!C:C,Moorings!B:B=A11,Moorings!D:D=D11))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="36">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="I11" s="37"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!A:A,Moorings!B:B=left(A12,14),Moorings!D:D=D12))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!A:A,Moorings!B:B=left(A12,14),Moorings!D:D=D12))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C12" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!C:C,Moorings!B:B=left(A12,14),Moorings!D:D=D12))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!C:C,Moorings!B:B=left(A12,14),Moorings!D:D=D12))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D12" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!A:A,Moorings!B:B=A12,Moorings!D:D=D12))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!A:A,Moorings!B:B=A12,Moorings!D:D=D12))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F12" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!C:C,Moorings!B:B=A12,Moorings!D:D=D12))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A12),"""",filter(Moorings!C:C,Moorings!B:B=A12,Moorings!D:D=D12))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G12" s="33" t="s">
         <v>53</v>
       </c>
       <c r="H12" s="36">
-        <v>0.0061</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="I12" s="37"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1">
       <c r="A13" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!A:A,Moorings!B:B=left(A13,14),Moorings!D:D=D13))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!A:A,Moorings!B:B=left(A13,14),Moorings!D:D=D13))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C13" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!C:C,Moorings!B:B=left(A13,14),Moorings!D:D=D13))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!C:C,Moorings!B:B=left(A13,14),Moorings!D:D=D13))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D13" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!A:A,Moorings!B:B=A13,Moorings!D:D=D13))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!A:A,Moorings!B:B=A13,Moorings!D:D=D13))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F13" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!C:C,Moorings!B:B=A13,Moorings!D:D=D13))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A13),"""",filter(Moorings!C:C,Moorings!B:B=A13,Moorings!D:D=D13))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>54</v>
       </c>
       <c r="H13" s="36">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="I13" s="37"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1">
       <c r="A14" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!A:A,Moorings!B:B=left(A14,14),Moorings!D:D=D14))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!A:A,Moorings!B:B=left(A14,14),Moorings!D:D=D14))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C14" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!C:C,Moorings!B:B=left(A14,14),Moorings!D:D=D14))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!C:C,Moorings!B:B=left(A14,14),Moorings!D:D=D14))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D14" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!A:A,Moorings!B:B=A14,Moorings!D:D=D14))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!A:A,Moorings!B:B=A14,Moorings!D:D=D14))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F14" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!C:C,Moorings!B:B=A14,Moorings!D:D=D14))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A14),"""",filter(Moorings!C:C,Moorings!B:B=A14,Moorings!D:D=D14))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G14" s="33" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="36">
-        <v>0.0121</v>
+        <v>1.21E-2</v>
       </c>
       <c r="I14" s="37"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1">
       <c r="A15" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!A:A,Moorings!B:B=left(A15,14),Moorings!D:D=D15))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!A:A,Moorings!B:B=left(A15,14),Moorings!D:D=D15))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C15" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!C:C,Moorings!B:B=left(A15,14),Moorings!D:D=D15))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!C:C,Moorings!B:B=left(A15,14),Moorings!D:D=D15))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D15" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!A:A,Moorings!B:B=A15,Moorings!D:D=D15))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!A:A,Moorings!B:B=A15,Moorings!D:D=D15))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F15" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!C:C,Moorings!B:B=A15,Moorings!D:D=D15))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A15),"""",filter(Moorings!C:C,Moorings!B:B=A15,Moorings!D:D=D15))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G15" s="33" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="36">
-        <v>117.0</v>
+        <v>140</v>
       </c>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!A:A,Moorings!B:B=left(A16,14),Moorings!D:D=D16))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!A:A,Moorings!B:B=left(A16,14),Moorings!D:D=D16))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C16" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!C:C,Moorings!B:B=left(A16,14),Moorings!D:D=D16))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!C:C,Moorings!B:B=left(A16,14),Moorings!D:D=D16))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D16" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!A:A,Moorings!B:B=A16,Moorings!D:D=D16))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!A:A,Moorings!B:B=A16,Moorings!D:D=D16))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F16" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!C:C,Moorings!B:B=A16,Moorings!D:D=D16))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A16),"""",filter(Moorings!C:C,Moorings!B:B=A16,Moorings!D:D=D16))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G16" s="33" t="s">
         <v>57</v>
       </c>
       <c r="H16" s="36">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="I16" s="37"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="A17" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!A:A,Moorings!B:B=left(A17,14),Moorings!D:D=D17))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!A:A,Moorings!B:B=left(A17,14),Moorings!D:D=D17))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C17" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!C:C,Moorings!B:B=left(A17,14),Moorings!D:D=D17))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!C:C,Moorings!B:B=left(A17,14),Moorings!D:D=D17))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D17" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!A:A,Moorings!B:B=A17,Moorings!D:D=D17))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!A:A,Moorings!B:B=A17,Moorings!D:D=D17))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F17" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!C:C,Moorings!B:B=A17,Moorings!D:D=D17))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!C:C,Moorings!B:B=A17,Moorings!D:D=D17))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="36">
-        <v>1.08</v>
+        <v>1.0960000000000001</v>
       </c>
       <c r="I17" s="37"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!A:A,Moorings!B:B=left(A18,14),Moorings!D:D=D18))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!A:A,Moorings!B:B=left(A18,14),Moorings!D:D=D18))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C18" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!C:C,Moorings!B:B=left(A18,14),Moorings!D:D=D18))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!C:C,Moorings!B:B=left(A18,14),Moorings!D:D=D18))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D18" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!A:A,Moorings!B:B=A18,Moorings!D:D=D18))"),"ATAPL-70110-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!A:A,Moorings!B:B=A18,Moorings!D:D=D18))"),"ATAPL-70110-00003")</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="F18" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!C:C,Moorings!B:B=A18,Moorings!D:D=D18))"),"3398")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!C:C,Moorings!B:B=A18,Moorings!D:D=D18))"),"3398")</f>
         <v>3398</v>
       </c>
       <c r="G18" s="33" t="s">
         <v>59</v>
       </c>
       <c r="H18" s="36">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I18" s="37"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" s="47"/>
       <c r="B19" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!A:A,Moorings!B:B=left(A19,14),Moorings!D:D=D19))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!A:A,Moorings!B:B=left(A19,14),Moorings!D:D=D19))"),"")</f>
         <v/>
       </c>
       <c r="C19" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!C:C,Moorings!B:B=left(A19,14),Moorings!D:D=D19))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!C:C,Moorings!B:B=left(A19,14),Moorings!D:D=D19))"),"")</f>
         <v/>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!A:A,Moorings!B:B=A19,Moorings!D:D=D19))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!A:A,Moorings!B:B=A19,Moorings!D:D=D19))"),"")</f>
         <v/>
       </c>
       <c r="F19" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!C:C,Moorings!B:B=A19,Moorings!D:D=D19))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!C:C,Moorings!B:B=A19,Moorings!D:D=D19))"),"")</f>
         <v/>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="36"/>
       <c r="I19" s="37"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!A:A,Moorings!B:B=left(A20,14),Moorings!D:D=D20))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!A:A,Moorings!B:B=left(A20,14),Moorings!D:D=D20))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C20" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!C:C,Moorings!B:B=left(A20,14),Moorings!D:D=D20))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!C:C,Moorings!B:B=left(A20,14),Moorings!D:D=D20))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D20" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!A:A,Moorings!B:B=A20,Moorings!D:D=D20))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!A:A,Moorings!B:B=A20,Moorings!D:D=D20))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F20" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!C:C,Moorings!B:B=A20,Moorings!D:D=D20))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!C:C,Moorings!B:B=A20,Moorings!D:D=D20))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G20" s="40" t="s">
         <v>52</v>
       </c>
       <c r="H20" s="43">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="I20" s="44"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="A21" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!A:A,Moorings!B:B=left(A21,14),Moorings!D:D=D21))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!A:A,Moorings!B:B=left(A21,14),Moorings!D:D=D21))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C21" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!C:C,Moorings!B:B=left(A21,14),Moorings!D:D=D21))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!C:C,Moorings!B:B=left(A21,14),Moorings!D:D=D21))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D21" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!A:A,Moorings!B:B=A21,Moorings!D:D=D21))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!A:A,Moorings!B:B=A21,Moorings!D:D=D21))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F21" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!C:C,Moorings!B:B=A21,Moorings!D:D=D21))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!C:C,Moorings!B:B=A21,Moorings!D:D=D21))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G21" s="40" t="s">
         <v>53</v>
       </c>
       <c r="H21" s="43">
-        <v>0.0061</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="I21" s="44"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="A22" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!A:A,Moorings!B:B=left(A22,14),Moorings!D:D=D22))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!A:A,Moorings!B:B=left(A22,14),Moorings!D:D=D22))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C22" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!C:C,Moorings!B:B=left(A22,14),Moorings!D:D=D22))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!C:C,Moorings!B:B=left(A22,14),Moorings!D:D=D22))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D22" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!A:A,Moorings!B:B=A22,Moorings!D:D=D22))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!A:A,Moorings!B:B=A22,Moorings!D:D=D22))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F22" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!C:C,Moorings!B:B=A22,Moorings!D:D=D22))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!C:C,Moorings!B:B=A22,Moorings!D:D=D22))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G22" s="40" t="s">
         <v>54</v>
       </c>
       <c r="H22" s="43">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="I22" s="44"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!A:A,Moorings!B:B=left(A23,14),Moorings!D:D=D23))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!A:A,Moorings!B:B=left(A23,14),Moorings!D:D=D23))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C23" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!C:C,Moorings!B:B=left(A23,14),Moorings!D:D=D23))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!C:C,Moorings!B:B=left(A23,14),Moorings!D:D=D23))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D23" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!A:A,Moorings!B:B=A23,Moorings!D:D=D23))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!A:A,Moorings!B:B=A23,Moorings!D:D=D23))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F23" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!C:C,Moorings!B:B=A23,Moorings!D:D=D23))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!C:C,Moorings!B:B=A23,Moorings!D:D=D23))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G23" s="40" t="s">
         <v>55</v>
       </c>
       <c r="H23" s="43">
-        <v>0.0121</v>
+        <v>1.21E-2</v>
       </c>
       <c r="I23" s="44"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="A24" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!A:A,Moorings!B:B=left(A24,14),Moorings!D:D=D24))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!A:A,Moorings!B:B=left(A24,14),Moorings!D:D=D24))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C24" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!C:C,Moorings!B:B=left(A24,14),Moorings!D:D=D24))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!C:C,Moorings!B:B=left(A24,14),Moorings!D:D=D24))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D24" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!A:A,Moorings!B:B=A24,Moorings!D:D=D24))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!A:A,Moorings!B:B=A24,Moorings!D:D=D24))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F24" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!C:C,Moorings!B:B=A24,Moorings!D:D=D24))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!C:C,Moorings!B:B=A24,Moorings!D:D=D24))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G24" s="40" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="43">
-        <v>117.0</v>
+        <v>140</v>
       </c>
       <c r="I24" s="44"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="A25" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!A:A,Moorings!B:B=left(A25,14),Moorings!D:D=D25))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!A:A,Moorings!B:B=left(A25,14),Moorings!D:D=D25))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C25" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!C:C,Moorings!B:B=left(A25,14),Moorings!D:D=D25))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!C:C,Moorings!B:B=left(A25,14),Moorings!D:D=D25))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D25" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!A:A,Moorings!B:B=A25,Moorings!D:D=D25))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!A:A,Moorings!B:B=A25,Moorings!D:D=D25))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F25" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!C:C,Moorings!B:B=A25,Moorings!D:D=D25))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!C:C,Moorings!B:B=A25,Moorings!D:D=D25))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G25" s="40" t="s">
         <v>57</v>
       </c>
       <c r="H25" s="43">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="I25" s="44"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="A26" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!A:A,Moorings!B:B=left(A26,14),Moorings!D:D=D26))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!A:A,Moorings!B:B=left(A26,14),Moorings!D:D=D26))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C26" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!C:C,Moorings!B:B=left(A26,14),Moorings!D:D=D26))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!C:C,Moorings!B:B=left(A26,14),Moorings!D:D=D26))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D26" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!A:A,Moorings!B:B=A26,Moorings!D:D=D26))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!A:A,Moorings!B:B=A26,Moorings!D:D=D26))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F26" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!C:C,Moorings!B:B=A26,Moorings!D:D=D26))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!C:C,Moorings!B:B=A26,Moorings!D:D=D26))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G26" s="40" t="s">
         <v>58</v>
       </c>
       <c r="H26" s="43">
-        <v>1.08</v>
+        <v>1.0960000000000001</v>
       </c>
       <c r="I26" s="44"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!A:A,Moorings!B:B=left(A27,14),Moorings!D:D=D27))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!A:A,Moorings!B:B=left(A27,14),Moorings!D:D=D27))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C27" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!C:C,Moorings!B:B=left(A27,14),Moorings!D:D=D27))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!C:C,Moorings!B:B=left(A27,14),Moorings!D:D=D27))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D27" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E27" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!A:A,Moorings!B:B=A27,Moorings!D:D=D27))"),"ATAPL-70110-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!A:A,Moorings!B:B=A27,Moorings!D:D=D27))"),"ATAPL-70110-00006")</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="F27" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!C:C,Moorings!B:B=A27,Moorings!D:D=D27))"),"3762")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!C:C,Moorings!B:B=A27,Moorings!D:D=D27))"),"3762")</f>
         <v>3762</v>
       </c>
       <c r="G27" s="40" t="s">
         <v>59</v>
       </c>
       <c r="H27" s="43">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I27" s="44"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="A28" s="33"/>
       <c r="B28" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!A:A,Moorings!B:B=left(A28,14),Moorings!D:D=D28))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!A:A,Moorings!B:B=left(A28,14),Moorings!D:D=D28))"),"")</f>
         <v/>
       </c>
       <c r="C28" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!C:C,Moorings!B:B=left(A28,14),Moorings!D:D=D28))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!C:C,Moorings!B:B=left(A28,14),Moorings!D:D=D28))"),"")</f>
         <v/>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!A:A,Moorings!B:B=A28,Moorings!D:D=D28))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!A:A,Moorings!B:B=A28,Moorings!D:D=D28))"),"")</f>
         <v/>
       </c>
       <c r="F28" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!C:C,Moorings!B:B=A28,Moorings!D:D=D28))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!C:C,Moorings!B:B=A28,Moorings!D:D=D28))"),"")</f>
         <v/>
       </c>
       <c r="G28" s="33"/>
       <c r="H28" s="50"/>
       <c r="I28" s="37"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!A:A,Moorings!B:B=left(A29,14),Moorings!D:D=D29))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!A:A,Moorings!B:B=left(A29,14),Moorings!D:D=D29))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C29" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!C:C,Moorings!B:B=left(A29,14),Moorings!D:D=D29))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!C:C,Moorings!B:B=left(A29,14),Moorings!D:D=D29))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D29" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!A:A,Moorings!B:B=A29,Moorings!D:D=D29))"),"ATAPL-70111-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!A:A,Moorings!B:B=A29,Moorings!D:D=D29))"),"ATAPL-70111-00003")</f>
         <v>ATAPL-70111-00003</v>
       </c>
       <c r="F29" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!C:C,Moorings!B:B=A29,Moorings!D:D=D29))"),"3400")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!C:C,Moorings!B:B=A29,Moorings!D:D=D29))"),"3400")</f>
         <v>3400</v>
       </c>
       <c r="G29" s="33" t="s">
         <v>60</v>
       </c>
       <c r="H29" s="52">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I29" s="37"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="A30" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!A:A,Moorings!B:B=left(A30,14),Moorings!D:D=D30))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!A:A,Moorings!B:B=left(A30,14),Moorings!D:D=D30))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C30" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!C:C,Moorings!B:B=left(A30,14),Moorings!D:D=D30))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!C:C,Moorings!B:B=left(A30,14),Moorings!D:D=D30))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D30" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!A:A,Moorings!B:B=A30,Moorings!D:D=D30))"),"ATAPL-70111-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!A:A,Moorings!B:B=A30,Moorings!D:D=D30))"),"ATAPL-70111-00003")</f>
         <v>ATAPL-70111-00003</v>
       </c>
       <c r="F30" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!C:C,Moorings!B:B=A30,Moorings!D:D=D30))"),"3400")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!C:C,Moorings!B:B=A30,Moorings!D:D=D30))"),"3400")</f>
         <v>3400</v>
       </c>
       <c r="G30" s="33" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="52">
-        <v>0.0303</v>
+        <v>3.0300000000000001E-2</v>
       </c>
       <c r="I30" s="37"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="A31" s="49"/>
       <c r="B31" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!A:A,Moorings!B:B=left(A31,14),Moorings!D:D=D31))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!A:A,Moorings!B:B=left(A31,14),Moorings!D:D=D31))"),"")</f>
         <v/>
       </c>
       <c r="C31" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!C:C,Moorings!B:B=left(A31,14),Moorings!D:D=D31))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!C:C,Moorings!B:B=left(A31,14),Moorings!D:D=D31))"),"")</f>
         <v/>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!A:A,Moorings!B:B=A31,Moorings!D:D=D31))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!A:A,Moorings!B:B=A31,Moorings!D:D=D31))"),"")</f>
         <v/>
       </c>
       <c r="F31" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!C:C,Moorings!B:B=A31,Moorings!D:D=D31))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!C:C,Moorings!B:B=A31,Moorings!D:D=D31))"),"")</f>
         <v/>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="36"/>
       <c r="I31" s="37"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="A32" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!A:A,Moorings!B:B=left(A32,14),Moorings!D:D=D32))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!A:A,Moorings!B:B=left(A32,14),Moorings!D:D=D32))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C32" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!C:C,Moorings!B:B=left(A32,14),Moorings!D:D=D32))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!C:C,Moorings!B:B=left(A32,14),Moorings!D:D=D32))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D32" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E32" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!A:A,Moorings!B:B=A32,Moorings!D:D=D32))"),"ATAPL-70111-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!A:A,Moorings!B:B=A32,Moorings!D:D=D32))"),"ATAPL-70111-00006")</f>
         <v>ATAPL-70111-00006</v>
       </c>
       <c r="F32" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!C:C,Moorings!B:B=A32,Moorings!D:D=D32))"),"3717")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!C:C,Moorings!B:B=A32,Moorings!D:D=D32))"),"3717")</f>
         <v>3717</v>
       </c>
       <c r="G32" s="40" t="s">
         <v>60</v>
       </c>
       <c r="H32" s="53">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
       <c r="A33" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!A:A,Moorings!B:B=left(A33,14),Moorings!D:D=D33))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!A:A,Moorings!B:B=left(A33,14),Moorings!D:D=D33))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C33" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!C:C,Moorings!B:B=left(A33,14),Moorings!D:D=D33))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!C:C,Moorings!B:B=left(A33,14),Moorings!D:D=D33))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D33" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E33" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!A:A,Moorings!B:B=A33,Moorings!D:D=D33))"),"ATAPL-70111-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!A:A,Moorings!B:B=A33,Moorings!D:D=D33))"),"ATAPL-70111-00006")</f>
         <v>ATAPL-70111-00006</v>
       </c>
       <c r="F33" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!C:C,Moorings!B:B=A33,Moorings!D:D=D33))"),"3717")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!C:C,Moorings!B:B=A33,Moorings!D:D=D33))"),"3717")</f>
         <v>3717</v>
       </c>
       <c r="G33" s="40" t="s">
         <v>61</v>
       </c>
       <c r="H33" s="53">
-        <v>0.0303</v>
+        <v>3.0300000000000001E-2</v>
       </c>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1">
       <c r="A34" s="47"/>
       <c r="B34" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!A:A,Moorings!B:B=left(A34,14),Moorings!D:D=D34))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!A:A,Moorings!B:B=left(A34,14),Moorings!D:D=D34))"),"")</f>
         <v/>
       </c>
       <c r="C34" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!C:C,Moorings!B:B=left(A34,14),Moorings!D:D=D34))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!C:C,Moorings!B:B=left(A34,14),Moorings!D:D=D34))"),"")</f>
         <v/>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!A:A,Moorings!B:B=A34,Moorings!D:D=D34))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!A:A,Moorings!B:B=A34,Moorings!D:D=D34))"),"")</f>
         <v/>
       </c>
       <c r="F34" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!C:C,Moorings!B:B=A34,Moorings!D:D=D34))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!C:C,Moorings!B:B=A34,Moorings!D:D=D34))"),"")</f>
         <v/>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="36"/>
       <c r="I34" s="37"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1">
       <c r="A35" s="33" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!A:A,Moorings!B:B=left(A35,14),Moorings!D:D=D35))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!A:A,Moorings!B:B=left(A35,14),Moorings!D:D=D35))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C35" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!C:C,Moorings!B:B=left(A35,14),Moorings!D:D=D35))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!C:C,Moorings!B:B=left(A35,14),Moorings!D:D=D35))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D35" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!A:A,Moorings!B:B=A35,Moorings!D:D=D35))"),"ATAPL-58346-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!A:A,Moorings!B:B=A35,Moorings!D:D=D35))"),"ATAPL-58346-00003")</f>
         <v>ATAPL-58346-00003</v>
       </c>
       <c r="F35" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!C:C,Moorings!B:B=A35,Moorings!D:D=D35))"),"1131")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!C:C,Moorings!B:B=A35,Moorings!D:D=D35))"),"1131")</f>
         <v>1131</v>
       </c>
       <c r="G35" s="35" t="s">
@@ -2442,27 +2919,27 @@
       </c>
       <c r="I35" s="37"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
       <c r="A36" s="33" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!A:A,Moorings!B:B=left(A36,14),Moorings!D:D=D36))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!A:A,Moorings!B:B=left(A36,14),Moorings!D:D=D36))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C36" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!C:C,Moorings!B:B=left(A36,14),Moorings!D:D=D36))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!C:C,Moorings!B:B=left(A36,14),Moorings!D:D=D36))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D36" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!A:A,Moorings!B:B=A36,Moorings!D:D=D36))"),"ATAPL-58346-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!A:A,Moorings!B:B=A36,Moorings!D:D=D36))"),"ATAPL-58346-00003")</f>
         <v>ATAPL-58346-00003</v>
       </c>
       <c r="F36" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!C:C,Moorings!B:B=A36,Moorings!D:D=D36))"),"1131")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!C:C,Moorings!B:B=A36,Moorings!D:D=D36))"),"1131")</f>
         <v>1131</v>
       </c>
       <c r="G36" s="35" t="s">
@@ -2473,27 +2950,27 @@
       </c>
       <c r="I36" s="37"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1">
       <c r="A37" s="33" t="s">
         <v>23</v>
       </c>
       <c r="B37" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!A:A,Moorings!B:B=left(A37,14),Moorings!D:D=D37))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!A:A,Moorings!B:B=left(A37,14),Moorings!D:D=D37))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C37" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!C:C,Moorings!B:B=left(A37,14),Moorings!D:D=D37))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!C:C,Moorings!B:B=left(A37,14),Moorings!D:D=D37))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D37" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!A:A,Moorings!B:B=A37,Moorings!D:D=D37))"),"ATAPL-58346-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!A:A,Moorings!B:B=A37,Moorings!D:D=D37))"),"ATAPL-58346-00003")</f>
         <v>ATAPL-58346-00003</v>
       </c>
       <c r="F37" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!C:C,Moorings!B:B=A37,Moorings!D:D=D37))"),"1131")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!C:C,Moorings!B:B=A37,Moorings!D:D=D37))"),"1131")</f>
         <v>1131</v>
       </c>
       <c r="G37" s="33" t="s">
@@ -2504,58 +2981,58 @@
       </c>
       <c r="I37" s="37"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
       <c r="A38" s="33" t="s">
         <v>23</v>
       </c>
       <c r="B38" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!A:A,Moorings!B:B=left(A38,14),Moorings!D:D=D38))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!A:A,Moorings!B:B=left(A38,14),Moorings!D:D=D38))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C38" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!C:C,Moorings!B:B=left(A38,14),Moorings!D:D=D38))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!C:C,Moorings!B:B=left(A38,14),Moorings!D:D=D38))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D38" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!A:A,Moorings!B:B=A38,Moorings!D:D=D38))"),"ATAPL-58346-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!A:A,Moorings!B:B=A38,Moorings!D:D=D38))"),"ATAPL-58346-00003")</f>
         <v>ATAPL-58346-00003</v>
       </c>
       <c r="F38" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!C:C,Moorings!B:B=A38,Moorings!D:D=D38))"),"1131")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!C:C,Moorings!B:B=A38,Moorings!D:D=D38))"),"1131")</f>
         <v>1131</v>
       </c>
       <c r="G38" s="33" t="s">
         <v>48</v>
       </c>
       <c r="H38" s="36">
-        <v>44.3682766666666</v>
+        <v>44.368276666666603</v>
       </c>
       <c r="I38" s="37"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
       <c r="A39" s="33" t="s">
         <v>23</v>
       </c>
       <c r="B39" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!A:A,Moorings!B:B=left(A39,14),Moorings!D:D=D39))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!A:A,Moorings!B:B=left(A39,14),Moorings!D:D=D39))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C39" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!C:C,Moorings!B:B=left(A39,14),Moorings!D:D=D39))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!C:C,Moorings!B:B=left(A39,14),Moorings!D:D=D39))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D39" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!A:A,Moorings!B:B=A39,Moorings!D:D=D39))"),"ATAPL-58346-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!A:A,Moorings!B:B=A39,Moorings!D:D=D39))"),"ATAPL-58346-00003")</f>
         <v>ATAPL-58346-00003</v>
       </c>
       <c r="F39" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!C:C,Moorings!B:B=A39,Moorings!D:D=D39))"),"1131")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A39),"""",filter(Moorings!C:C,Moorings!B:B=A39,Moorings!D:D=D39))"),"1131")</f>
         <v>1131</v>
       </c>
       <c r="G39" s="33" t="s">
@@ -2566,50 +3043,50 @@
       </c>
       <c r="I39" s="37"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
       <c r="A40" s="47"/>
       <c r="B40" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!A:A,Moorings!B:B=left(A40,14),Moorings!D:D=D40))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!A:A,Moorings!B:B=left(A40,14),Moorings!D:D=D40))"),"")</f>
         <v/>
       </c>
       <c r="C40" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!C:C,Moorings!B:B=left(A40,14),Moorings!D:D=D40))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!C:C,Moorings!B:B=left(A40,14),Moorings!D:D=D40))"),"")</f>
         <v/>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!A:A,Moorings!B:B=A40,Moorings!D:D=D40))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!A:A,Moorings!B:B=A40,Moorings!D:D=D40))"),"")</f>
         <v/>
       </c>
       <c r="F40" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!C:C,Moorings!B:B=A40,Moorings!D:D=D40))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!C:C,Moorings!B:B=A40,Moorings!D:D=D40))"),"")</f>
         <v/>
       </c>
       <c r="G40" s="33"/>
       <c r="H40" s="48"/>
       <c r="I40" s="37"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
       <c r="A41" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B41" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!A:A,Moorings!B:B=left(A41,14),Moorings!D:D=D41))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!A:A,Moorings!B:B=left(A41,14),Moorings!D:D=D41))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C41" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!C:C,Moorings!B:B=left(A41,14),Moorings!D:D=D41))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!C:C,Moorings!B:B=left(A41,14),Moorings!D:D=D41))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D41" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E41" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!A:A,Moorings!B:B=A41,Moorings!D:D=D41))"),"ATAPL-58346-00007")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!A:A,Moorings!B:B=A41,Moorings!D:D=D41))"),"ATAPL-58346-00007")</f>
         <v>ATAPL-58346-00007</v>
       </c>
       <c r="F41" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!C:C,Moorings!B:B=A41,Moorings!D:D=D41))"),"1216")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!C:C,Moorings!B:B=A41,Moorings!D:D=D41))"),"1216")</f>
         <v>1216</v>
       </c>
       <c r="G41" s="42" t="s">
@@ -2620,27 +3097,27 @@
       </c>
       <c r="I41" s="44"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1">
       <c r="A42" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!A:A,Moorings!B:B=left(A42,14),Moorings!D:D=D42))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!A:A,Moorings!B:B=left(A42,14),Moorings!D:D=D42))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C42" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!C:C,Moorings!B:B=left(A42,14),Moorings!D:D=D42))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!C:C,Moorings!B:B=left(A42,14),Moorings!D:D=D42))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D42" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!A:A,Moorings!B:B=A42,Moorings!D:D=D42))"),"ATAPL-58346-00007")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!A:A,Moorings!B:B=A42,Moorings!D:D=D42))"),"ATAPL-58346-00007")</f>
         <v>ATAPL-58346-00007</v>
       </c>
       <c r="F42" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!C:C,Moorings!B:B=A42,Moorings!D:D=D42))"),"1216")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A42),"""",filter(Moorings!C:C,Moorings!B:B=A42,Moorings!D:D=D42))"),"1216")</f>
         <v>1216</v>
       </c>
       <c r="G42" s="42" t="s">
@@ -2651,27 +3128,27 @@
       </c>
       <c r="I42" s="44"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
       <c r="A43" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!A:A,Moorings!B:B=left(A43,14),Moorings!D:D=D43))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!A:A,Moorings!B:B=left(A43,14),Moorings!D:D=D43))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C43" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!C:C,Moorings!B:B=left(A43,14),Moorings!D:D=D43))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!C:C,Moorings!B:B=left(A43,14),Moorings!D:D=D43))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D43" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E43" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!A:A,Moorings!B:B=A43,Moorings!D:D=D43))"),"ATAPL-58346-00007")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!A:A,Moorings!B:B=A43,Moorings!D:D=D43))"),"ATAPL-58346-00007")</f>
         <v>ATAPL-58346-00007</v>
       </c>
       <c r="F43" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!C:C,Moorings!B:B=A43,Moorings!D:D=D43))"),"1216")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A43),"""",filter(Moorings!C:C,Moorings!B:B=A43,Moorings!D:D=D43))"),"1216")</f>
         <v>1216</v>
       </c>
       <c r="G43" s="40" t="s">
@@ -2682,58 +3159,58 @@
       </c>
       <c r="I43" s="44"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
       <c r="A44" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!A:A,Moorings!B:B=left(A44,14),Moorings!D:D=D44))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!A:A,Moorings!B:B=left(A44,14),Moorings!D:D=D44))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C44" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!C:C,Moorings!B:B=left(A44,14),Moorings!D:D=D44))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!C:C,Moorings!B:B=left(A44,14),Moorings!D:D=D44))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D44" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E44" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!A:A,Moorings!B:B=A44,Moorings!D:D=D44))"),"ATAPL-58346-00007")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!A:A,Moorings!B:B=A44,Moorings!D:D=D44))"),"ATAPL-58346-00007")</f>
         <v>ATAPL-58346-00007</v>
       </c>
       <c r="F44" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!C:C,Moorings!B:B=A44,Moorings!D:D=D44))"),"1216")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A44),"""",filter(Moorings!C:C,Moorings!B:B=A44,Moorings!D:D=D44))"),"1216")</f>
         <v>1216</v>
       </c>
       <c r="G44" s="40" t="s">
         <v>48</v>
       </c>
       <c r="H44" s="43">
-        <v>44.3682766666666</v>
+        <v>44.368276666666603</v>
       </c>
       <c r="I44" s="44"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
       <c r="A45" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!A:A,Moorings!B:B=left(A45,14),Moorings!D:D=D45))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!A:A,Moorings!B:B=left(A45,14),Moorings!D:D=D45))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C45" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!C:C,Moorings!B:B=left(A45,14),Moorings!D:D=D45))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!C:C,Moorings!B:B=left(A45,14),Moorings!D:D=D45))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D45" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E45" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!A:A,Moorings!B:B=A45,Moorings!D:D=D45))"),"ATAPL-58346-00007")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!A:A,Moorings!B:B=A45,Moorings!D:D=D45))"),"ATAPL-58346-00007")</f>
         <v>ATAPL-58346-00007</v>
       </c>
       <c r="F45" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!C:C,Moorings!B:B=A45,Moorings!D:D=D45))"),"1216")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A45),"""",filter(Moorings!C:C,Moorings!B:B=A45,Moorings!D:D=D45))"),"1216")</f>
         <v>1216</v>
       </c>
       <c r="G45" s="40" t="s">
@@ -2744,81 +3221,81 @@
       </c>
       <c r="I45" s="44"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1">
       <c r="A46" s="47"/>
       <c r="B46" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!A:A,Moorings!B:B=left(A46,14),Moorings!D:D=D46))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!A:A,Moorings!B:B=left(A46,14),Moorings!D:D=D46))"),"")</f>
         <v/>
       </c>
       <c r="C46" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!C:C,Moorings!B:B=left(A46,14),Moorings!D:D=D46))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!C:C,Moorings!B:B=left(A46,14),Moorings!D:D=D46))"),"")</f>
         <v/>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!A:A,Moorings!B:B=A46,Moorings!D:D=D46))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!A:A,Moorings!B:B=A46,Moorings!D:D=D46))"),"")</f>
         <v/>
       </c>
       <c r="F46" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!C:C,Moorings!B:B=A46,Moorings!D:D=D46))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!C:C,Moorings!B:B=A46,Moorings!D:D=D46))"),"")</f>
         <v/>
       </c>
       <c r="G46" s="33"/>
       <c r="H46" s="48"/>
       <c r="I46" s="37"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1">
       <c r="A47" s="33" t="s">
         <v>20</v>
       </c>
       <c r="B47" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!A:A,Moorings!B:B=left(A47,14),Moorings!D:D=D47))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!A:A,Moorings!B:B=left(A47,14),Moorings!D:D=D47))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C47" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!C:C,Moorings!B:B=left(A47,14),Moorings!D:D=D47))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!C:C,Moorings!B:B=left(A47,14),Moorings!D:D=D47))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D47" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!A:A,Moorings!B:B=A47,Moorings!D:D=D47))"),"ATAPL-67977-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!A:A,Moorings!B:B=A47,Moorings!D:D=D47))"),"ATAPL-67977-00003")</f>
         <v>ATAPL-67977-00003</v>
       </c>
       <c r="F47" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!C:C,Moorings!B:B=A47,Moorings!D:D=D47))"),"5277187-0138")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!C:C,Moorings!B:B=A47,Moorings!D:D=D47))"),"5277187-0138")</f>
         <v>5277187-0138</v>
       </c>
       <c r="G47" s="33" t="s">
         <v>48</v>
       </c>
       <c r="H47" s="48">
-        <v>44.3682766666666</v>
+        <v>44.368276666666603</v>
       </c>
       <c r="I47" s="37"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1">
       <c r="A48" s="33" t="s">
         <v>20</v>
       </c>
       <c r="B48" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!A:A,Moorings!B:B=left(A48,14),Moorings!D:D=D48))"),"ATAPL-71403-00004")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!A:A,Moorings!B:B=left(A48,14),Moorings!D:D=D48))"),"ATAPL-71403-00004")</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="C48" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!C:C,Moorings!B:B=left(A48,14),Moorings!D:D=D48))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!C:C,Moorings!B:B=left(A48,14),Moorings!D:D=D48))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D48" s="16">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!A:A,Moorings!B:B=A48,Moorings!D:D=D48))"),"ATAPL-67977-00003")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!A:A,Moorings!B:B=A48,Moorings!D:D=D48))"),"ATAPL-67977-00003")</f>
         <v>ATAPL-67977-00003</v>
       </c>
       <c r="F48" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!C:C,Moorings!B:B=A48,Moorings!D:D=D48))"),"5277187-0138")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!C:C,Moorings!B:B=A48,Moorings!D:D=D48))"),"5277187-0138")</f>
         <v>5277187-0138</v>
       </c>
       <c r="G48" s="33" t="s">
@@ -2829,81 +3306,81 @@
       </c>
       <c r="I48" s="37"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1">
       <c r="A49" s="47"/>
       <c r="B49" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!A:A,Moorings!B:B=left(A49,14),Moorings!D:D=D49))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!A:A,Moorings!B:B=left(A49,14),Moorings!D:D=D49))"),"")</f>
         <v/>
       </c>
       <c r="C49" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!C:C,Moorings!B:B=left(A49,14),Moorings!D:D=D49))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!C:C,Moorings!B:B=left(A49,14),Moorings!D:D=D49))"),"")</f>
         <v/>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!A:A,Moorings!B:B=A49,Moorings!D:D=D49))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!A:A,Moorings!B:B=A49,Moorings!D:D=D49))"),"")</f>
         <v/>
       </c>
       <c r="F49" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!C:C,Moorings!B:B=A49,Moorings!D:D=D49))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!C:C,Moorings!B:B=A49,Moorings!D:D=D49))"),"")</f>
         <v/>
       </c>
       <c r="G49" s="33"/>
       <c r="H49" s="36"/>
       <c r="I49" s="37"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1">
       <c r="A50" s="40" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!A:A,Moorings!B:B=left(A50,14),Moorings!D:D=D50))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!A:A,Moorings!B:B=left(A50,14),Moorings!D:D=D50))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C50" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!C:C,Moorings!B:B=left(A50,14),Moorings!D:D=D50))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!C:C,Moorings!B:B=left(A50,14),Moorings!D:D=D50))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D50" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E50" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!A:A,Moorings!B:B=A50,Moorings!D:D=D50))"),"ATAPL-67977-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!A:A,Moorings!B:B=A50,Moorings!D:D=D50))"),"ATAPL-67977-00006")</f>
         <v>ATAPL-67977-00006</v>
       </c>
       <c r="F50" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!C:C,Moorings!B:B=A50,Moorings!D:D=D50))"),"52-0146")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A50),"""",filter(Moorings!C:C,Moorings!B:B=A50,Moorings!D:D=D50))"),"52-0146")</f>
         <v>52-0146</v>
       </c>
       <c r="G50" s="40" t="s">
         <v>48</v>
       </c>
       <c r="H50" s="54">
-        <v>44.3682766666666</v>
+        <v>44.368276666666603</v>
       </c>
       <c r="I50" s="44"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1">
       <c r="A51" s="40" t="s">
         <v>20</v>
       </c>
       <c r="B51" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!A:A,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"ATAPL-71403-00005")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!A:A,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"ATAPL-71403-00005")</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="C51" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!C:C,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"CE04OSPD-DP01B-00001")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!C:C,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"CE04OSPD-DP01B-00001")</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
       <c r="D51" s="41">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E51" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!A:A,Moorings!B:B=A51,Moorings!D:D=D51))"),"ATAPL-67977-00006")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!A:A,Moorings!B:B=A51,Moorings!D:D=D51))"),"ATAPL-67977-00006")</f>
         <v>ATAPL-67977-00006</v>
       </c>
       <c r="F51" s="34" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!C:C,Moorings!B:B=A51,Moorings!D:D=D51))"),"52-0146")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!C:C,Moorings!B:B=A51,Moorings!D:D=D51))"),"52-0146")</f>
         <v>52-0146</v>
       </c>
       <c r="G51" s="40" t="s">
@@ -2914,46 +3391,46 @@
       </c>
       <c r="I51" s="44"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:9" ht="15.75" customHeight="1">
       <c r="A52" s="47"/>
       <c r="B52" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!A:A,Moorings!B:B=left(A52,14),Moorings!D:D=D52))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!A:A,Moorings!B:B=left(A52,14),Moorings!D:D=D52))"),"")</f>
         <v/>
       </c>
       <c r="C52" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!C:C,Moorings!B:B=left(A52,14),Moorings!D:D=D52))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!C:C,Moorings!B:B=left(A52,14),Moorings!D:D=D52))"),"")</f>
         <v/>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!A:A,Moorings!B:B=A52,Moorings!D:D=D52))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!A:A,Moorings!B:B=A52,Moorings!D:D=D52))"),"")</f>
         <v/>
       </c>
       <c r="F52" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!C:C,Moorings!B:B=A52,Moorings!D:D=D52))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!C:C,Moorings!B:B=A52,Moorings!D:D=D52))"),"")</f>
         <v/>
       </c>
       <c r="G52" s="33"/>
       <c r="H52" s="36"/>
       <c r="I52" s="37"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" spans="1:9" ht="15.75" customHeight="1">
       <c r="A53" s="47"/>
       <c r="B53" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
         <v/>
       </c>
       <c r="C53" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!C:C,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!C:C,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
         <v/>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=A53,Moorings!D:D=D53))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=A53,Moorings!D:D=D53))"),"")</f>
         <v/>
       </c>
       <c r="F53" s="30" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!C:C,Moorings!B:B=A53,Moorings!D:D=D53))"),"")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!C:C,Moorings!B:B=A53,Moorings!D:D=D53))"),"")</f>
         <v/>
       </c>
       <c r="G53" s="33"/>
@@ -2961,31 +3438,38 @@
       <c r="I53" s="37"/>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.86"/>
-    <col customWidth="1" min="2" max="2" width="17.14"/>
-    <col customWidth="1" min="3" max="3" width="31.57"/>
-    <col customWidth="1" min="4" max="4" width="7.71"/>
-    <col customWidth="1" min="5" max="5" width="21.71"/>
-    <col customWidth="1" min="6" max="6" width="9.86"/>
-    <col customWidth="1" min="7" max="7" width="11.43"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="55" t="s">
         <v>68</v>
       </c>
@@ -3008,48 +3492,48 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7">
       <c r="A2" s="57" t="str">
         <f>Moorings!A2</f>
         <v>ATAPL-71403-00004</v>
       </c>
       <c r="B2" s="57" t="str">
-        <f>if(D2="Mooring",Moorings!B2,"")</f>
+        <f>IF(D2="Mooring",Moorings!B2,"")</f>
         <v>CE04OSPD-DP01B</v>
       </c>
       <c r="C2" s="58" t="str">
-        <f>if(D2="Sensor",Moorings!B2,"")</f>
+        <f>IF(D2="Sensor",Moorings!B2,"")</f>
         <v/>
       </c>
       <c r="D2" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B2),"",if(len(Moorings!B2)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B2),"",IF(LEN(Moorings!B2)&gt;14,"Sensor","Mooring"))</f>
         <v>Mooring</v>
       </c>
       <c r="E2" s="34" t="str">
         <f>Moorings!C2</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
-      <c r="F2" s="59" t="str">
-        <f>if(D2="Mooring",Moorings!E2,"")</f>
-        <v>8/16/2014</v>
+      <c r="F2" s="59">
+        <f>IF(D2="Mooring",Moorings!E2,"")</f>
+        <v>41867</v>
       </c>
       <c r="G2" s="58"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7">
       <c r="A3" s="57" t="str">
         <f>Moorings!A3</f>
         <v>ATAPL-67977-00003</v>
       </c>
       <c r="B3" s="57" t="str">
-        <f>if(D3="Mooring",Moorings!B3,"")</f>
+        <f>IF(D3="Mooring",Moorings!B3,"")</f>
         <v/>
       </c>
       <c r="C3" s="57" t="str">
-        <f>if(D3="Sensor",Moorings!B3,"")</f>
+        <f>IF(D3="Sensor",Moorings!B3,"")</f>
         <v>CE04OSPD-DP01B-01-CTDPFL105</v>
       </c>
       <c r="D3" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B3),"",if(len(Moorings!B3)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B3),"",IF(LEN(Moorings!B3)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
       <c r="E3" s="34" t="str">
@@ -3057,188 +3541,188 @@
         <v>5277187-0138</v>
       </c>
       <c r="F3" s="59" t="str">
-        <f>if(D3="Mooring",Moorings!E3,"")</f>
+        <f>IF(D3="Mooring",Moorings!E3,"")</f>
         <v/>
       </c>
       <c r="G3" s="58"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7">
       <c r="A4" s="57" t="str">
         <f>Moorings!A4</f>
         <v>ATAPL-58346-00003</v>
       </c>
       <c r="B4" s="57" t="str">
-        <f>if(D4="Mooring",Moorings!B4,"")</f>
+        <f>IF(D4="Mooring",Moorings!B4,"")</f>
         <v/>
       </c>
       <c r="C4" s="57" t="str">
-        <f>if(D4="Sensor",Moorings!B4,"")</f>
+        <f>IF(D4="Sensor",Moorings!B4,"")</f>
         <v>CE04OSPD-DP01B-02-VEL3DA105</v>
       </c>
       <c r="D4" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B4),"",if(len(Moorings!B4)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B4),"",IF(LEN(Moorings!B4)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E4" s="34" t="str">
+      <c r="E4" s="34">
         <f>Moorings!C4</f>
         <v>1131</v>
       </c>
       <c r="F4" s="59" t="str">
-        <f>if(D4="Mooring",Moorings!E4,"")</f>
+        <f>IF(D4="Mooring",Moorings!E4,"")</f>
         <v/>
       </c>
       <c r="G4" s="58"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7">
       <c r="A5" s="57" t="str">
         <f>Moorings!A5</f>
         <v>ATAPL-70111-00003</v>
       </c>
       <c r="B5" s="57" t="str">
-        <f>if(D5="Mooring",Moorings!B5,"")</f>
+        <f>IF(D5="Mooring",Moorings!B5,"")</f>
         <v/>
       </c>
       <c r="C5" s="57" t="str">
-        <f>if(D5="Sensor",Moorings!B5,"")</f>
+        <f>IF(D5="Sensor",Moorings!B5,"")</f>
         <v>CE04OSPD-DP01B-03-FLCDRA103</v>
       </c>
       <c r="D5" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B5),"",if(len(Moorings!B5)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B5),"",IF(LEN(Moorings!B5)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E5" s="34" t="str">
+      <c r="E5" s="34">
         <f>Moorings!C5</f>
         <v>3400</v>
       </c>
       <c r="F5" s="59" t="str">
-        <f>if(D5="Mooring",Moorings!E5,"")</f>
+        <f>IF(D5="Mooring",Moorings!E5,"")</f>
         <v/>
       </c>
       <c r="G5" s="58"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7">
       <c r="A6" s="57" t="str">
         <f>Moorings!A6</f>
         <v>ATAPL-70110-00003</v>
       </c>
       <c r="B6" s="57" t="str">
-        <f>if(D6="Mooring",Moorings!B6,"")</f>
+        <f>IF(D6="Mooring",Moorings!B6,"")</f>
         <v/>
       </c>
       <c r="C6" s="57" t="str">
-        <f>if(D6="Sensor",Moorings!B6,"")</f>
+        <f>IF(D6="Sensor",Moorings!B6,"")</f>
         <v>CE04OSPD-DP01B-04-FLNTUA103</v>
       </c>
       <c r="D6" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B6),"",if(len(Moorings!B6)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B6),"",IF(LEN(Moorings!B6)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E6" s="34" t="str">
+      <c r="E6" s="34">
         <f>Moorings!C6</f>
         <v>3398</v>
       </c>
       <c r="F6" s="59" t="str">
-        <f>if(D6="Mooring",Moorings!E6,"")</f>
+        <f>IF(D6="Mooring",Moorings!E6,"")</f>
         <v/>
       </c>
       <c r="G6" s="58"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7">
       <c r="A7" s="57" t="str">
         <f>Moorings!A7</f>
         <v>A00175</v>
       </c>
       <c r="B7" s="57" t="str">
-        <f>if(D7="Mooring",Moorings!B7,"")</f>
+        <f>IF(D7="Mooring",Moorings!B7,"")</f>
         <v/>
       </c>
       <c r="C7" s="57" t="str">
-        <f>if(D7="Sensor",Moorings!B7,"")</f>
+        <f>IF(D7="Sensor",Moorings!B7,"")</f>
         <v>CE04OSPD-DP01B-06-DOSTAD105</v>
       </c>
       <c r="D7" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B7),"",if(len(Moorings!B7)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B7),"",IF(LEN(Moorings!B7)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E7" s="34" t="str">
+      <c r="E7" s="34">
         <f>Moorings!C7</f>
         <v>137</v>
       </c>
       <c r="F7" s="59" t="str">
-        <f>if(D7="Mooring",Moorings!E7,"")</f>
+        <f>IF(D7="Mooring",Moorings!E7,"")</f>
         <v/>
       </c>
       <c r="G7" s="58"/>
     </row>
-    <row r="8">
-      <c r="A8" s="57" t="str">
+    <row r="8" spans="1:7">
+      <c r="A8" s="57">
         <f>Moorings!A8</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B8" s="57" t="str">
-        <f>if(D8="Mooring",Moorings!B8,"")</f>
+        <f>IF(D8="Mooring",Moorings!B8,"")</f>
         <v/>
       </c>
       <c r="C8" s="58" t="str">
-        <f>if(D8="Sensor",Moorings!B8,"")</f>
+        <f>IF(D8="Sensor",Moorings!B8,"")</f>
         <v/>
       </c>
       <c r="D8" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B8),"",if(len(Moorings!B8)&gt;14,"Sensor","Mooring"))</f>
-        <v/>
-      </c>
-      <c r="E8" s="34" t="str">
+        <f>IF(ISBLANK(Moorings!B8),"",IF(LEN(Moorings!B8)&gt;14,"Sensor","Mooring"))</f>
+        <v/>
+      </c>
+      <c r="E8" s="34">
         <f>Moorings!C8</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="F8" s="59" t="str">
-        <f>if(D8="Mooring",Moorings!E8,"")</f>
+        <f>IF(D8="Mooring",Moorings!E8,"")</f>
         <v/>
       </c>
       <c r="G8" s="58"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7">
       <c r="A9" s="57" t="str">
         <f>Moorings!A9</f>
         <v>ATAPL-71403-00005</v>
       </c>
       <c r="B9" s="57" t="str">
-        <f>if(D9="Mooring",Moorings!B9,"")</f>
+        <f>IF(D9="Mooring",Moorings!B9,"")</f>
         <v>CE04OSPD-DP01B</v>
       </c>
       <c r="C9" s="58" t="str">
-        <f>if(D9="Sensor",Moorings!B9,"")</f>
+        <f>IF(D9="Sensor",Moorings!B9,"")</f>
         <v/>
       </c>
       <c r="D9" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B9),"",if(len(Moorings!B9)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B9),"",IF(LEN(Moorings!B9)&gt;14,"Sensor","Mooring"))</f>
         <v>Mooring</v>
       </c>
       <c r="E9" s="34" t="str">
         <f>Moorings!C9</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
-      <c r="F9" s="59" t="str">
-        <f>if(D9="Mooring",Moorings!E9,"")</f>
-        <v>7/24/2015</v>
+      <c r="F9" s="59">
+        <f>IF(D9="Mooring",Moorings!E9,"")</f>
+        <v>42209</v>
       </c>
       <c r="G9" s="58"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7">
       <c r="A10" s="57" t="str">
         <f>Moorings!A10</f>
         <v>ATAPL-67977-00006</v>
       </c>
       <c r="B10" s="57" t="str">
-        <f>if(D10="Mooring",Moorings!B10,"")</f>
+        <f>IF(D10="Mooring",Moorings!B10,"")</f>
         <v/>
       </c>
       <c r="C10" s="57" t="str">
-        <f>if(D10="Sensor",Moorings!B10,"")</f>
+        <f>IF(D10="Sensor",Moorings!B10,"")</f>
         <v>CE04OSPD-DP01B-01-CTDPFL105</v>
       </c>
       <c r="D10" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B10),"",if(len(Moorings!B10)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B10),"",IF(LEN(Moorings!B10)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
       <c r="E10" s="34" t="str">
@@ -3246,196 +3730,202 @@
         <v>52-0146</v>
       </c>
       <c r="F10" s="59" t="str">
-        <f>if(D10="Mooring",Moorings!E10,"")</f>
+        <f>IF(D10="Mooring",Moorings!E10,"")</f>
         <v/>
       </c>
       <c r="G10" s="58"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7">
       <c r="A11" s="57" t="str">
         <f>Moorings!A11</f>
         <v>ATAPL-58346-00007</v>
       </c>
       <c r="B11" s="57" t="str">
-        <f>if(D11="Mooring",Moorings!B11,"")</f>
+        <f>IF(D11="Mooring",Moorings!B11,"")</f>
         <v/>
       </c>
       <c r="C11" s="57" t="str">
-        <f>if(D11="Sensor",Moorings!B11,"")</f>
+        <f>IF(D11="Sensor",Moorings!B11,"")</f>
         <v>CE04OSPD-DP01B-02-VEL3DA105</v>
       </c>
       <c r="D11" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B11),"",if(len(Moorings!B11)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B11),"",IF(LEN(Moorings!B11)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E11" s="34" t="str">
+      <c r="E11" s="34">
         <f>Moorings!C11</f>
         <v>1216</v>
       </c>
       <c r="F11" s="59" t="str">
-        <f>if(D11="Mooring",Moorings!E11,"")</f>
+        <f>IF(D11="Mooring",Moorings!E11,"")</f>
         <v/>
       </c>
       <c r="G11" s="58"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7">
       <c r="A12" s="57" t="str">
         <f>Moorings!A12</f>
         <v>ATAPL-70111-00006</v>
       </c>
       <c r="B12" s="57" t="str">
-        <f>if(D12="Mooring",Moorings!B12,"")</f>
+        <f>IF(D12="Mooring",Moorings!B12,"")</f>
         <v/>
       </c>
       <c r="C12" s="57" t="str">
-        <f>if(D12="Sensor",Moorings!B12,"")</f>
+        <f>IF(D12="Sensor",Moorings!B12,"")</f>
         <v>CE04OSPD-DP01B-03-FLCDRA103</v>
       </c>
       <c r="D12" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B12),"",if(len(Moorings!B12)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B12),"",IF(LEN(Moorings!B12)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E12" s="34" t="str">
+      <c r="E12" s="34">
         <f>Moorings!C12</f>
         <v>3717</v>
       </c>
       <c r="F12" s="59" t="str">
-        <f>if(D12="Mooring",Moorings!E12,"")</f>
+        <f>IF(D12="Mooring",Moorings!E12,"")</f>
         <v/>
       </c>
       <c r="G12" s="58"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7">
       <c r="A13" s="57" t="str">
         <f>Moorings!A13</f>
         <v>ATAPL-70110-00006</v>
       </c>
       <c r="B13" s="57" t="str">
-        <f>if(D13="Mooring",Moorings!B13,"")</f>
+        <f>IF(D13="Mooring",Moorings!B13,"")</f>
         <v/>
       </c>
       <c r="C13" s="57" t="str">
-        <f>if(D13="Sensor",Moorings!B13,"")</f>
+        <f>IF(D13="Sensor",Moorings!B13,"")</f>
         <v>CE04OSPD-DP01B-04-FLNTUA103</v>
       </c>
       <c r="D13" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B13),"",if(len(Moorings!B13)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B13),"",IF(LEN(Moorings!B13)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E13" s="34" t="str">
+      <c r="E13" s="34">
         <f>Moorings!C13</f>
         <v>3762</v>
       </c>
       <c r="F13" s="59" t="str">
-        <f>if(D13="Mooring",Moorings!E13,"")</f>
+        <f>IF(D13="Mooring",Moorings!E13,"")</f>
         <v/>
       </c>
       <c r="G13" s="58"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7">
       <c r="A14" s="57" t="str">
         <f>Moorings!A14</f>
         <v>ATOSU-58320-00018</v>
       </c>
       <c r="B14" s="57" t="str">
-        <f>if(D14="Mooring",Moorings!B14,"")</f>
+        <f>IF(D14="Mooring",Moorings!B14,"")</f>
         <v/>
       </c>
       <c r="C14" s="57" t="str">
-        <f>if(D14="Sensor",Moorings!B14,"")</f>
+        <f>IF(D14="Sensor",Moorings!B14,"")</f>
         <v>CE04OSPD-DP01B-06-DOSTAD105</v>
       </c>
       <c r="D14" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B14),"",if(len(Moorings!B14)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B14),"",IF(LEN(Moorings!B14)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E14" s="34" t="str">
+      <c r="E14" s="34">
         <f>Moorings!C14</f>
         <v>317</v>
       </c>
       <c r="F14" s="59" t="str">
-        <f>if(D14="Mooring",Moorings!E14,"")</f>
+        <f>IF(D14="Mooring",Moorings!E14,"")</f>
         <v/>
       </c>
       <c r="G14" s="58"/>
     </row>
-    <row r="15">
-      <c r="A15" s="57" t="str">
+    <row r="15" spans="1:7">
+      <c r="A15" s="57">
         <f>Moorings!A15</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B15" s="57" t="str">
-        <f>if(D15="Mooring",Moorings!B15,"")</f>
+        <f>IF(D15="Mooring",Moorings!B15,"")</f>
         <v/>
       </c>
       <c r="C15" s="58" t="str">
-        <f>if(D15="Sensor",Moorings!B15,"")</f>
+        <f>IF(D15="Sensor",Moorings!B15,"")</f>
         <v/>
       </c>
       <c r="D15" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B15),"",if(len(Moorings!B15)&gt;14,"Sensor","Mooring"))</f>
-        <v/>
-      </c>
-      <c r="E15" s="34" t="str">
+        <f>IF(ISBLANK(Moorings!B15),"",IF(LEN(Moorings!B15)&gt;14,"Sensor","Mooring"))</f>
+        <v/>
+      </c>
+      <c r="E15" s="34">
         <f>Moorings!C15</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="F15" s="59" t="str">
-        <f>if(D15="Mooring",Moorings!E15,"")</f>
+        <f>IF(D15="Mooring",Moorings!E15,"")</f>
         <v/>
       </c>
       <c r="G15" s="58"/>
     </row>
-    <row r="16">
-      <c r="A16" s="57" t="str">
+    <row r="16" spans="1:7">
+      <c r="A16" s="57">
         <f>Moorings!A16</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B16" s="57" t="str">
-        <f>if(D16="Mooring",Moorings!B16,"")</f>
+        <f>IF(D16="Mooring",Moorings!B16,"")</f>
         <v/>
       </c>
       <c r="C16" s="58" t="str">
-        <f>if(D16="Sensor",Moorings!B16,"")</f>
+        <f>IF(D16="Sensor",Moorings!B16,"")</f>
         <v/>
       </c>
       <c r="D16" s="30" t="str">
-        <f>if(ISBLANK(Moorings!B16),"",if(len(Moorings!B16)&gt;14,"Sensor","Mooring"))</f>
-        <v/>
-      </c>
-      <c r="E16" s="34" t="str">
+        <f>IF(ISBLANK(Moorings!B16),"",IF(LEN(Moorings!B16)&gt;14,"Sensor","Mooring"))</f>
+        <v/>
+      </c>
+      <c r="E16" s="34">
         <f>Moorings!C16</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="F16" s="59" t="str">
-        <f>if(D16="Mooring",Moorings!E16,"")</f>
+        <f>IF(D16="Mooring",Moorings!E16,"")</f>
         <v/>
       </c>
       <c r="G16" s="58"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="33.43"/>
-    <col customWidth="1" min="2" max="2" width="11.57"/>
-    <col customWidth="1" min="3" max="3" width="14.86"/>
-    <col customWidth="1" min="4" max="6" width="11.0"/>
-    <col customWidth="1" min="7" max="7" width="5.71"/>
-    <col customWidth="1" min="8" max="8" width="16.0"/>
-    <col customWidth="1" min="9" max="9" width="19.43"/>
-    <col customWidth="1" min="10" max="10" width="11.0"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11">
       <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
@@ -3465,7 +3955,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3487,7 +3977,7 @@
       <c r="I2" s="67"/>
       <c r="J2" s="66"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3509,7 +3999,7 @@
       <c r="I3" s="68"/>
       <c r="J3" s="64"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3531,7 +4021,7 @@
       <c r="I4" s="68"/>
       <c r="J4" s="66"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3553,7 +4043,7 @@
       <c r="I5" s="67"/>
       <c r="J5" s="66"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -3575,7 +4065,7 @@
       <c r="I6" s="68"/>
       <c r="J6" s="66"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3597,7 +4087,7 @@
       <c r="I7" s="68"/>
       <c r="J7" s="66"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="B8" s="69"/>
       <c r="C8" s="69"/>
       <c r="D8" s="70"/>
@@ -3608,7 +4098,7 @@
       <c r="I8" s="67"/>
       <c r="J8" s="66"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="B9" s="64"/>
       <c r="C9" s="65"/>
       <c r="D9" s="64"/>
@@ -3619,7 +4109,7 @@
       <c r="I9" s="68"/>
       <c r="J9" s="66"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="B10" s="64"/>
       <c r="C10" s="65"/>
       <c r="D10" s="64"/>
@@ -3630,7 +4120,7 @@
       <c r="I10" s="68"/>
       <c r="J10" s="66"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="B11" s="64"/>
       <c r="C11" s="71"/>
       <c r="D11" s="66"/>
@@ -3641,7 +4131,7 @@
       <c r="I11" s="67"/>
       <c r="J11" s="66"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="B12" s="64"/>
       <c r="C12" s="65"/>
       <c r="D12" s="64"/>
@@ -3654,7 +4144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="B13" s="64"/>
       <c r="C13" s="71"/>
       <c r="D13" s="64"/>
@@ -3668,7 +4158,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
       <c r="D14" s="64"/>
@@ -3682,7 +4172,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="B15" s="64"/>
       <c r="C15" s="65"/>
       <c r="D15" s="64"/>
@@ -3696,7 +4186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="B16" s="64"/>
       <c r="C16" s="65"/>
       <c r="D16" s="64"/>
@@ -3710,7 +4200,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:11" ht="15" customHeight="1">
       <c r="B17" s="64"/>
       <c r="C17" s="65"/>
       <c r="D17" s="64"/>
@@ -3724,7 +4214,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:11" ht="15" customHeight="1">
       <c r="B18" s="64"/>
       <c r="C18" s="65"/>
       <c r="D18" s="64"/>
@@ -3738,7 +4228,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="2:11" ht="15" customHeight="1">
       <c r="B19" s="64"/>
       <c r="C19" s="65"/>
       <c r="D19" s="64"/>
@@ -3752,21 +4242,21 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="2:11" ht="15" customHeight="1">
       <c r="B20" s="69" t="str">
-        <f>concatenate(countif(B2:B19,"yes"),"/",counta(B2:B19))</f>
+        <f>CONCATENATE(COUNTIF(B2:B19,"yes"),"/",COUNTA(B2:B19))</f>
         <v>6/6</v>
       </c>
       <c r="C20" s="69" t="str">
-        <f>concatenate("'",countif(C2:C19,"yes"),"/",counta(C2:C19))</f>
+        <f>CONCATENATE("'",COUNTIF(C2:C19,"yes"),"/",COUNTA(C2:C19))</f>
         <v>'0/6</v>
       </c>
       <c r="D20" s="70" t="str">
-        <f t="shared" ref="D20:E20" si="1">concatenate("'",countif(D2:D19,"1/*")+countif(D2:D19,"2/*")*2,"/",countif(D2:D19,"*/1")+countif(D2:D19,"*/2")*2)</f>
+        <f t="shared" ref="D20:E20" si="0">CONCATENATE("'",COUNTIF(D2:D19,"1/*")+COUNTIF(D2:D19,"2/*")*2,"/",COUNTIF(D2:D19,"*/1")+COUNTIF(D2:D19,"*/2")*2)</f>
         <v>'12/12</v>
       </c>
       <c r="E20" s="70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>'10/10</v>
       </c>
       <c r="F20" s="66"/>
@@ -3778,7 +4268,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="2:11" ht="15" customHeight="1">
       <c r="B21" s="66"/>
       <c r="C21" s="65"/>
       <c r="D21" s="64"/>
@@ -3792,7 +4282,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="2:11" ht="15" customHeight="1">
       <c r="B22" s="66"/>
       <c r="C22" s="71"/>
       <c r="D22" s="66"/>
@@ -3806,7 +4296,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="2:11" ht="15" customHeight="1">
       <c r="B23" s="66"/>
       <c r="C23" s="71"/>
       <c r="D23" s="66"/>
@@ -3820,7 +4310,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:11" ht="15" customHeight="1">
       <c r="B24" s="66"/>
       <c r="C24" s="71"/>
       <c r="D24" s="66"/>
@@ -3834,7 +4324,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="2:11" ht="15" customHeight="1">
       <c r="B25" s="66"/>
       <c r="C25" s="71"/>
       <c r="D25" s="66"/>
@@ -3849,7 +4339,13 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added OOI Bar Codes, corrected reference designators
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE04OSPD.xlsx
+++ b/deployment/Omaha_Cal_Info_CE04OSPD.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="940" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9675" yWindow="945" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="IntegrationEvents" sheetId="3" r:id="rId3"/>
     <sheet name="Verification" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,26 +32,28 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>equipment list as ATAPL-58320, but that is too short
 	-Dan Mergens</t>
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>equipment list shows 137
 bulk load has 215
@@ -54,65 +61,70 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0">
+    <comment ref="E20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>missing from bulk load
 	-Dan Mergens</t>
         </r>
       </text>
     </comment>
-    <comment ref="E32" authorId="0">
+    <comment ref="E32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>missing from bulk load
 	-Dan Mergens</t>
         </r>
       </text>
     </comment>
-    <comment ref="H32" authorId="0">
+    <comment ref="H32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>not sure if these calibration values were for the first or second deployment - just duplicated them - applies to all instruments
 	-Dan Mergens</t>
         </r>
       </text>
     </comment>
-    <comment ref="E41" authorId="0">
+    <comment ref="E41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>missing from bulk load
 	-Dan Mergens</t>
         </r>
       </text>
     </comment>
-    <comment ref="E50" authorId="0">
+    <comment ref="E50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>missing from bulk load
 	-Dan Mergens</t>
@@ -129,13 +141,14 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>no data, so it doesn't show up in the UI with a name :(
 	-Dan Mergens</t>
@@ -147,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="92">
   <si>
     <t>Mooring OOIBARCODE</t>
   </si>
@@ -410,6 +423,24 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>CE04OSPD-DP01B-00-ENG000000</t>
+  </si>
+  <si>
+    <t>CE04OSPD-DP01B-04-FLCDRA103</t>
+  </si>
+  <si>
+    <t>CE04OSPD-DP01B-ENG-00001</t>
+  </si>
+  <si>
+    <t>CE04OSPD-DP01B-ENG-00002</t>
+  </si>
+  <si>
+    <t>OL000575</t>
+  </si>
+  <si>
+    <t>OL000576</t>
   </si>
 </sst>
 </file>
@@ -421,7 +452,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="166" formatCode="m&quot;/&quot;d&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -430,34 +461,47 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF999999"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -528,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -662,9 +706,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -719,12 +760,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -781,6 +834,97 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 7" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8839200" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -834,6 +978,97 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1164,23 +1399,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="E30:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="7" width="12" customWidth="1"/>
-    <col min="8" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" customWidth="1"/>
-    <col min="13" max="14" width="14.5" customWidth="1"/>
+    <col min="8" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="14" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27" customHeight="1">
+    <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1455,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1239,7 +1474,9 @@
       <c r="F2" s="8">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9">
+        <v>42208</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>15</v>
       </c>
@@ -1264,7 +1501,7 @@
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
@@ -1283,7 +1520,9 @@
       <c r="F3" s="8">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="9">
+        <v>42208</v>
+      </c>
       <c r="H3" s="17" t="s">
         <v>15</v>
       </c>
@@ -1308,7 +1547,7 @@
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>22</v>
       </c>
@@ -1327,7 +1566,9 @@
       <c r="F4" s="8">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9">
+        <v>42208</v>
+      </c>
       <c r="H4" s="17" t="s">
         <v>15</v>
       </c>
@@ -1352,12 +1593,12 @@
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>25</v>
+      <c r="B5" t="s">
+        <v>87</v>
       </c>
       <c r="C5" s="16">
         <v>3400</v>
@@ -1371,7 +1612,9 @@
       <c r="F5" s="8">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="9">
+        <v>42208</v>
+      </c>
       <c r="H5" s="17" t="s">
         <v>15</v>
       </c>
@@ -1396,7 +1639,7 @@
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1415,7 +1658,9 @@
       <c r="F6" s="8">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>42208</v>
+      </c>
       <c r="H6" s="17" t="s">
         <v>15</v>
       </c>
@@ -1440,7 +1685,7 @@
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -1459,7 +1704,9 @@
       <c r="F7" s="8">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9">
+        <v>42208</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1484,7 +1731,7 @@
         <v>-124.95276</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1500,7 +1747,7 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>30</v>
       </c>
@@ -1544,7 +1791,7 @@
         <v>-124.95279666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1">
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>35</v>
       </c>
@@ -1588,7 +1835,7 @@
         <v>-124.95279666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="12.75" customHeight="1">
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>38</v>
       </c>
@@ -1632,12 +1879,12 @@
         <v>-124.95279666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="12.75" customHeight="1">
+    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>25</v>
+      <c r="B12" t="s">
+        <v>87</v>
       </c>
       <c r="C12" s="10">
         <v>3717</v>
@@ -1676,7 +1923,7 @@
         <v>-124.95279666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="12.75" customHeight="1">
+    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>40</v>
       </c>
@@ -1720,7 +1967,7 @@
         <v>-124.95279666666667</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="12.75" customHeight="1">
+    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>42</v>
       </c>
@@ -1764,7 +2011,7 @@
         <v>-124.95279666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1">
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
@@ -1780,7 +2027,7 @@
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
     </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1">
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
@@ -1796,7 +2043,7 @@
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
     </row>
-    <row r="17" spans="1:14" ht="12.75" customHeight="1">
+    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -1812,7 +2059,7 @@
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
     </row>
-    <row r="18" spans="1:14" ht="12.75" customHeight="1">
+    <row r="18" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -1828,7 +2075,7 @@
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
     </row>
-    <row r="19" spans="1:14" ht="12.75" customHeight="1">
+    <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -1844,7 +2091,7 @@
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
     </row>
-    <row r="20" spans="1:14" ht="12.75" customHeight="1">
+    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -1872,27 +2119,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53:E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.83203125" customWidth="1"/>
-    <col min="8" max="8" width="59.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1921,7 +2168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!A:A,Moorings!B:B=left(A2,14),Moorings!D:D=D2))"),"")</f>
@@ -1944,7 +2191,7 @@
       <c r="H2" s="31"/>
       <c r="I2" s="32"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>29</v>
       </c>
@@ -1975,7 +2222,7 @@
       </c>
       <c r="I3" s="37"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>29</v>
       </c>
@@ -2006,7 +2253,7 @@
       </c>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>29</v>
       </c>
@@ -2037,7 +2284,7 @@
       </c>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
       <c r="B6" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A6),"""",filter(Moorings!A:A,Moorings!B:B=left(A6,14),Moorings!D:D=D6))"),"")</f>
@@ -2060,7 +2307,7 @@
       <c r="H6" s="36"/>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>29</v>
       </c>
@@ -2091,7 +2338,7 @@
       </c>
       <c r="I7" s="44"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>29</v>
       </c>
@@ -2122,7 +2369,7 @@
       </c>
       <c r="I8" s="44"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>29</v>
       </c>
@@ -2153,7 +2400,7 @@
       </c>
       <c r="I9" s="42"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A10),"""",filter(Moorings!A:A,Moorings!B:B=left(A10,14),Moorings!D:D=D10))"),"")</f>
@@ -2176,7 +2423,7 @@
       <c r="H10" s="48"/>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>27</v>
       </c>
@@ -2207,7 +2454,7 @@
       </c>
       <c r="I11" s="37"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>27</v>
       </c>
@@ -2238,7 +2485,7 @@
       </c>
       <c r="I12" s="37"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>27</v>
       </c>
@@ -2269,7 +2516,7 @@
       </c>
       <c r="I13" s="37"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
         <v>27</v>
       </c>
@@ -2300,7 +2547,7 @@
       </c>
       <c r="I14" s="37"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
         <v>27</v>
       </c>
@@ -2331,7 +2578,7 @@
       </c>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
         <v>27</v>
       </c>
@@ -2362,7 +2609,7 @@
       </c>
       <c r="I16" s="37"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>27</v>
       </c>
@@ -2393,7 +2640,7 @@
       </c>
       <c r="I17" s="37"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
         <v>27</v>
       </c>
@@ -2424,7 +2671,7 @@
       </c>
       <c r="I18" s="37"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!A:A,Moorings!B:B=left(A19,14),Moorings!D:D=D19))"),"")</f>
@@ -2447,7 +2694,7 @@
       <c r="H19" s="36"/>
       <c r="I19" s="37"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
         <v>27</v>
       </c>
@@ -2478,7 +2725,7 @@
       </c>
       <c r="I20" s="44"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>27</v>
       </c>
@@ -2509,7 +2756,7 @@
       </c>
       <c r="I21" s="44"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
         <v>27</v>
       </c>
@@ -2540,7 +2787,7 @@
       </c>
       <c r="I22" s="44"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
         <v>27</v>
       </c>
@@ -2571,7 +2818,7 @@
       </c>
       <c r="I23" s="44"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
         <v>27</v>
       </c>
@@ -2602,7 +2849,7 @@
       </c>
       <c r="I24" s="44"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
         <v>27</v>
       </c>
@@ -2633,7 +2880,7 @@
       </c>
       <c r="I25" s="44"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
         <v>27</v>
       </c>
@@ -2664,7 +2911,7 @@
       </c>
       <c r="I26" s="44"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
         <v>27</v>
       </c>
@@ -2695,7 +2942,7 @@
       </c>
       <c r="I27" s="44"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!A:A,Moorings!B:B=left(A28,14),Moorings!D:D=D28))"),"")</f>
@@ -2718,9 +2965,9 @@
       <c r="H28" s="50"/>
       <c r="I28" s="37"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="51" t="s">
-        <v>25</v>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
       </c>
       <c r="B29" s="34" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!A:A,Moorings!B:B=left(A29,14),Moorings!D:D=D29))"),"ATAPL-71403-00004")</f>
@@ -2744,14 +2991,14 @@
       <c r="G29" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="52">
+      <c r="H29" s="51">
         <v>39</v>
       </c>
       <c r="I29" s="37"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="51" t="s">
-        <v>25</v>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>87</v>
       </c>
       <c r="B30" s="34" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!A:A,Moorings!B:B=left(A30,14),Moorings!D:D=D30))"),"ATAPL-71403-00004")</f>
@@ -2775,12 +3022,12 @@
       <c r="G30" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H30" s="52">
+      <c r="H30" s="51">
         <v>3.0300000000000001E-2</v>
       </c>
       <c r="I30" s="37"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!A:A,Moorings!B:B=left(A31,14),Moorings!D:D=D31))"),"")</f>
@@ -2803,9 +3050,9 @@
       <c r="H31" s="36"/>
       <c r="I31" s="37"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="51" t="s">
-        <v>25</v>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>87</v>
       </c>
       <c r="B32" s="34" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!A:A,Moorings!B:B=left(A32,14),Moorings!D:D=D32))"),"ATAPL-71403-00005")</f>
@@ -2829,14 +3076,14 @@
       <c r="G32" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="53">
+      <c r="H32" s="52">
         <v>39</v>
       </c>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A33" s="51" t="s">
-        <v>25</v>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>87</v>
       </c>
       <c r="B33" s="34" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!A:A,Moorings!B:B=left(A33,14),Moorings!D:D=D33))"),"ATAPL-71403-00005")</f>
@@ -2860,12 +3107,12 @@
       <c r="G33" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="H33" s="53">
+      <c r="H33" s="52">
         <v>3.0300000000000001E-2</v>
       </c>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!A:A,Moorings!B:B=left(A34,14),Moorings!D:D=D34))"),"")</f>
@@ -2888,7 +3135,7 @@
       <c r="H34" s="36"/>
       <c r="I34" s="37"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>23</v>
       </c>
@@ -2919,7 +3166,7 @@
       </c>
       <c r="I35" s="37"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>23</v>
       </c>
@@ -2950,7 +3197,7 @@
       </c>
       <c r="I36" s="37"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
         <v>23</v>
       </c>
@@ -2981,7 +3228,7 @@
       </c>
       <c r="I37" s="37"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>23</v>
       </c>
@@ -3012,7 +3259,7 @@
       </c>
       <c r="I38" s="37"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
         <v>23</v>
       </c>
@@ -3043,7 +3290,7 @@
       </c>
       <c r="I39" s="37"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
       <c r="B40" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A40),"""",filter(Moorings!A:A,Moorings!B:B=left(A40,14),Moorings!D:D=D40))"),"")</f>
@@ -3066,7 +3313,7 @@
       <c r="H40" s="48"/>
       <c r="I40" s="37"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
         <v>23</v>
       </c>
@@ -3097,7 +3344,7 @@
       </c>
       <c r="I41" s="44"/>
     </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
         <v>23</v>
       </c>
@@ -3128,7 +3375,7 @@
       </c>
       <c r="I42" s="44"/>
     </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
         <v>23</v>
       </c>
@@ -3159,7 +3406,7 @@
       </c>
       <c r="I43" s="44"/>
     </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
         <v>23</v>
       </c>
@@ -3190,7 +3437,7 @@
       </c>
       <c r="I44" s="44"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
         <v>23</v>
       </c>
@@ -3221,7 +3468,7 @@
       </c>
       <c r="I45" s="44"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1">
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47"/>
       <c r="B46" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A46),"""",filter(Moorings!A:A,Moorings!B:B=left(A46,14),Moorings!D:D=D46))"),"")</f>
@@ -3244,7 +3491,7 @@
       <c r="H46" s="48"/>
       <c r="I46" s="37"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1">
+    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>20</v>
       </c>
@@ -3275,7 +3522,7 @@
       </c>
       <c r="I47" s="37"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1">
+    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>20</v>
       </c>
@@ -3306,7 +3553,7 @@
       </c>
       <c r="I48" s="37"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" customHeight="1">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47"/>
       <c r="B49" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A49),"""",filter(Moorings!A:A,Moorings!B:B=left(A49,14),Moorings!D:D=D49))"),"")</f>
@@ -3329,7 +3576,7 @@
       <c r="H49" s="36"/>
       <c r="I49" s="37"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
         <v>20</v>
       </c>
@@ -3355,12 +3602,12 @@
       <c r="G50" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H50" s="54">
+      <c r="H50" s="53">
         <v>44.368276666666603</v>
       </c>
       <c r="I50" s="44"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
         <v>20</v>
       </c>
@@ -3391,7 +3638,7 @@
       </c>
       <c r="I51" s="44"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" customHeight="1">
+    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="47"/>
       <c r="B52" s="30" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A52),"""",filter(Moorings!A:A,Moorings!B:B=left(A52,14),Moorings!D:D=D52))"),"")</f>
@@ -3414,28 +3661,52 @@
       <c r="H52" s="36"/>
       <c r="I52" s="37"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A53" s="47"/>
-      <c r="B53" s="30" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
-        <v/>
-      </c>
-      <c r="C53" s="30" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!C:C,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
-        <v/>
-      </c>
-      <c r="D53" s="16"/>
-      <c r="E53" s="30" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=A53,Moorings!D:D=D53))"),"")</f>
-        <v/>
-      </c>
-      <c r="F53" s="30" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!C:C,Moorings!B:B=A53,Moorings!D:D=D53))"),"")</f>
-        <v/>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="34" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A48),"""",filter(Moorings!A:A,Moorings!B:B=left(A48,14),Moorings!D:D=D48))"),"ATAPL-71403-00004")</f>
+        <v>ATAPL-71403-00004</v>
+      </c>
+      <c r="C53" s="34" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!C:C,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"CE04OSPD-DP01B-00001")</f>
+        <v>CE04OSPD-DP01B-00001</v>
+      </c>
+      <c r="D53" s="16">
+        <v>1</v>
+      </c>
+      <c r="E53" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="73" t="s">
+        <v>88</v>
       </c>
       <c r="G53" s="33"/>
       <c r="H53" s="36"/>
       <c r="I53" s="37"/>
+    </row>
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="34" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!A:A,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"ATAPL-71403-00005")</f>
+        <v>ATAPL-71403-00005</v>
+      </c>
+      <c r="C54" s="34" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A51),"""",filter(Moorings!C:C,Moorings!B:B=left(A51,14),Moorings!D:D=D51))"),"CE04OSPD-DP01B-00001")</f>
+        <v>CE04OSPD-DP01B-00001</v>
+      </c>
+      <c r="D54" s="39">
+        <v>2</v>
+      </c>
+      <c r="E54" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="F54" s="73" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3458,50 +3729,50 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="31.5" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="55" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="57" t="str">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="str">
         <f>Moorings!A2</f>
         <v>ATAPL-71403-00004</v>
       </c>
-      <c r="B2" s="57" t="str">
+      <c r="B2" s="56" t="str">
         <f>IF(D2="Mooring",Moorings!B2,"")</f>
         <v>CE04OSPD-DP01B</v>
       </c>
-      <c r="C2" s="58" t="str">
+      <c r="C2" s="57" t="str">
         <f>IF(D2="Sensor",Moorings!B2,"")</f>
         <v/>
       </c>
@@ -3513,22 +3784,22 @@
         <f>Moorings!C2</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
-      <c r="F2" s="59">
+      <c r="F2" s="58">
         <f>IF(D2="Mooring",Moorings!E2,"")</f>
         <v>41867</v>
       </c>
-      <c r="G2" s="58"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="57" t="str">
+      <c r="G2" s="57"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="str">
         <f>Moorings!A3</f>
         <v>ATAPL-67977-00003</v>
       </c>
-      <c r="B3" s="57" t="str">
+      <c r="B3" s="56" t="str">
         <f>IF(D3="Mooring",Moorings!B3,"")</f>
         <v/>
       </c>
-      <c r="C3" s="57" t="str">
+      <c r="C3" s="56" t="str">
         <f>IF(D3="Sensor",Moorings!B3,"")</f>
         <v>CE04OSPD-DP01B-01-CTDPFL105</v>
       </c>
@@ -3540,22 +3811,22 @@
         <f>Moorings!C3</f>
         <v>5277187-0138</v>
       </c>
-      <c r="F3" s="59" t="str">
+      <c r="F3" s="58" t="str">
         <f>IF(D3="Mooring",Moorings!E3,"")</f>
         <v/>
       </c>
-      <c r="G3" s="58"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="57" t="str">
+      <c r="G3" s="57"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="str">
         <f>Moorings!A4</f>
         <v>ATAPL-58346-00003</v>
       </c>
-      <c r="B4" s="57" t="str">
+      <c r="B4" s="56" t="str">
         <f>IF(D4="Mooring",Moorings!B4,"")</f>
         <v/>
       </c>
-      <c r="C4" s="57" t="str">
+      <c r="C4" s="56" t="str">
         <f>IF(D4="Sensor",Moorings!B4,"")</f>
         <v>CE04OSPD-DP01B-02-VEL3DA105</v>
       </c>
@@ -3567,24 +3838,24 @@
         <f>Moorings!C4</f>
         <v>1131</v>
       </c>
-      <c r="F4" s="59" t="str">
+      <c r="F4" s="58" t="str">
         <f>IF(D4="Mooring",Moorings!E4,"")</f>
         <v/>
       </c>
-      <c r="G4" s="58"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="57" t="str">
+      <c r="G4" s="57"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="str">
         <f>Moorings!A5</f>
         <v>ATAPL-70111-00003</v>
       </c>
-      <c r="B5" s="57" t="str">
+      <c r="B5" s="56" t="str">
         <f>IF(D5="Mooring",Moorings!B5,"")</f>
         <v/>
       </c>
-      <c r="C5" s="57" t="str">
+      <c r="C5" s="56" t="str">
         <f>IF(D5="Sensor",Moorings!B5,"")</f>
-        <v>CE04OSPD-DP01B-03-FLCDRA103</v>
+        <v>CE04OSPD-DP01B-04-FLCDRA103</v>
       </c>
       <c r="D5" s="30" t="str">
         <f>IF(ISBLANK(Moorings!B5),"",IF(LEN(Moorings!B5)&gt;14,"Sensor","Mooring"))</f>
@@ -3594,22 +3865,22 @@
         <f>Moorings!C5</f>
         <v>3400</v>
       </c>
-      <c r="F5" s="59" t="str">
+      <c r="F5" s="58" t="str">
         <f>IF(D5="Mooring",Moorings!E5,"")</f>
         <v/>
       </c>
-      <c r="G5" s="58"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="57" t="str">
+      <c r="G5" s="57"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="str">
         <f>Moorings!A6</f>
         <v>ATAPL-70110-00003</v>
       </c>
-      <c r="B6" s="57" t="str">
+      <c r="B6" s="56" t="str">
         <f>IF(D6="Mooring",Moorings!B6,"")</f>
         <v/>
       </c>
-      <c r="C6" s="57" t="str">
+      <c r="C6" s="56" t="str">
         <f>IF(D6="Sensor",Moorings!B6,"")</f>
         <v>CE04OSPD-DP01B-04-FLNTUA103</v>
       </c>
@@ -3621,22 +3892,22 @@
         <f>Moorings!C6</f>
         <v>3398</v>
       </c>
-      <c r="F6" s="59" t="str">
+      <c r="F6" s="58" t="str">
         <f>IF(D6="Mooring",Moorings!E6,"")</f>
         <v/>
       </c>
-      <c r="G6" s="58"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="57" t="str">
+      <c r="G6" s="57"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="str">
         <f>Moorings!A7</f>
         <v>A00175</v>
       </c>
-      <c r="B7" s="57" t="str">
+      <c r="B7" s="56" t="str">
         <f>IF(D7="Mooring",Moorings!B7,"")</f>
         <v/>
       </c>
-      <c r="C7" s="57" t="str">
+      <c r="C7" s="56" t="str">
         <f>IF(D7="Sensor",Moorings!B7,"")</f>
         <v>CE04OSPD-DP01B-06-DOSTAD105</v>
       </c>
@@ -3648,22 +3919,22 @@
         <f>Moorings!C7</f>
         <v>137</v>
       </c>
-      <c r="F7" s="59" t="str">
+      <c r="F7" s="58" t="str">
         <f>IF(D7="Mooring",Moorings!E7,"")</f>
         <v/>
       </c>
-      <c r="G7" s="58"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="57">
+      <c r="G7" s="57"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="56">
         <f>Moorings!A8</f>
         <v>0</v>
       </c>
-      <c r="B8" s="57" t="str">
+      <c r="B8" s="56" t="str">
         <f>IF(D8="Mooring",Moorings!B8,"")</f>
         <v/>
       </c>
-      <c r="C8" s="58" t="str">
+      <c r="C8" s="57" t="str">
         <f>IF(D8="Sensor",Moorings!B8,"")</f>
         <v/>
       </c>
@@ -3675,22 +3946,22 @@
         <f>Moorings!C8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="59" t="str">
+      <c r="F8" s="58" t="str">
         <f>IF(D8="Mooring",Moorings!E8,"")</f>
         <v/>
       </c>
-      <c r="G8" s="58"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="57" t="str">
+      <c r="G8" s="57"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="str">
         <f>Moorings!A9</f>
         <v>ATAPL-71403-00005</v>
       </c>
-      <c r="B9" s="57" t="str">
+      <c r="B9" s="56" t="str">
         <f>IF(D9="Mooring",Moorings!B9,"")</f>
         <v>CE04OSPD-DP01B</v>
       </c>
-      <c r="C9" s="58" t="str">
+      <c r="C9" s="57" t="str">
         <f>IF(D9="Sensor",Moorings!B9,"")</f>
         <v/>
       </c>
@@ -3702,22 +3973,22 @@
         <f>Moorings!C9</f>
         <v>CE04OSPD-DP01B-00001</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="58">
         <f>IF(D9="Mooring",Moorings!E9,"")</f>
         <v>42209</v>
       </c>
-      <c r="G9" s="58"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="57" t="str">
+      <c r="G9" s="57"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="str">
         <f>Moorings!A10</f>
         <v>ATAPL-67977-00006</v>
       </c>
-      <c r="B10" s="57" t="str">
+      <c r="B10" s="56" t="str">
         <f>IF(D10="Mooring",Moorings!B10,"")</f>
         <v/>
       </c>
-      <c r="C10" s="57" t="str">
+      <c r="C10" s="56" t="str">
         <f>IF(D10="Sensor",Moorings!B10,"")</f>
         <v>CE04OSPD-DP01B-01-CTDPFL105</v>
       </c>
@@ -3729,22 +4000,22 @@
         <f>Moorings!C10</f>
         <v>52-0146</v>
       </c>
-      <c r="F10" s="59" t="str">
+      <c r="F10" s="58" t="str">
         <f>IF(D10="Mooring",Moorings!E10,"")</f>
         <v/>
       </c>
-      <c r="G10" s="58"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="57" t="str">
+      <c r="G10" s="57"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="str">
         <f>Moorings!A11</f>
         <v>ATAPL-58346-00007</v>
       </c>
-      <c r="B11" s="57" t="str">
+      <c r="B11" s="56" t="str">
         <f>IF(D11="Mooring",Moorings!B11,"")</f>
         <v/>
       </c>
-      <c r="C11" s="57" t="str">
+      <c r="C11" s="56" t="str">
         <f>IF(D11="Sensor",Moorings!B11,"")</f>
         <v>CE04OSPD-DP01B-02-VEL3DA105</v>
       </c>
@@ -3756,24 +4027,24 @@
         <f>Moorings!C11</f>
         <v>1216</v>
       </c>
-      <c r="F11" s="59" t="str">
+      <c r="F11" s="58" t="str">
         <f>IF(D11="Mooring",Moorings!E11,"")</f>
         <v/>
       </c>
-      <c r="G11" s="58"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="57" t="str">
+      <c r="G11" s="57"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="str">
         <f>Moorings!A12</f>
         <v>ATAPL-70111-00006</v>
       </c>
-      <c r="B12" s="57" t="str">
+      <c r="B12" s="56" t="str">
         <f>IF(D12="Mooring",Moorings!B12,"")</f>
         <v/>
       </c>
-      <c r="C12" s="57" t="str">
+      <c r="C12" s="56" t="str">
         <f>IF(D12="Sensor",Moorings!B12,"")</f>
-        <v>CE04OSPD-DP01B-03-FLCDRA103</v>
+        <v>CE04OSPD-DP01B-04-FLCDRA103</v>
       </c>
       <c r="D12" s="30" t="str">
         <f>IF(ISBLANK(Moorings!B12),"",IF(LEN(Moorings!B12)&gt;14,"Sensor","Mooring"))</f>
@@ -3783,22 +4054,22 @@
         <f>Moorings!C12</f>
         <v>3717</v>
       </c>
-      <c r="F12" s="59" t="str">
+      <c r="F12" s="58" t="str">
         <f>IF(D12="Mooring",Moorings!E12,"")</f>
         <v/>
       </c>
-      <c r="G12" s="58"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="57" t="str">
+      <c r="G12" s="57"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="str">
         <f>Moorings!A13</f>
         <v>ATAPL-70110-00006</v>
       </c>
-      <c r="B13" s="57" t="str">
+      <c r="B13" s="56" t="str">
         <f>IF(D13="Mooring",Moorings!B13,"")</f>
         <v/>
       </c>
-      <c r="C13" s="57" t="str">
+      <c r="C13" s="56" t="str">
         <f>IF(D13="Sensor",Moorings!B13,"")</f>
         <v>CE04OSPD-DP01B-04-FLNTUA103</v>
       </c>
@@ -3810,22 +4081,22 @@
         <f>Moorings!C13</f>
         <v>3762</v>
       </c>
-      <c r="F13" s="59" t="str">
+      <c r="F13" s="58" t="str">
         <f>IF(D13="Mooring",Moorings!E13,"")</f>
         <v/>
       </c>
-      <c r="G13" s="58"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="57" t="str">
+      <c r="G13" s="57"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="str">
         <f>Moorings!A14</f>
         <v>ATOSU-58320-00018</v>
       </c>
-      <c r="B14" s="57" t="str">
+      <c r="B14" s="56" t="str">
         <f>IF(D14="Mooring",Moorings!B14,"")</f>
         <v/>
       </c>
-      <c r="C14" s="57" t="str">
+      <c r="C14" s="56" t="str">
         <f>IF(D14="Sensor",Moorings!B14,"")</f>
         <v>CE04OSPD-DP01B-06-DOSTAD105</v>
       </c>
@@ -3837,22 +4108,22 @@
         <f>Moorings!C14</f>
         <v>317</v>
       </c>
-      <c r="F14" s="59" t="str">
+      <c r="F14" s="58" t="str">
         <f>IF(D14="Mooring",Moorings!E14,"")</f>
         <v/>
       </c>
-      <c r="G14" s="58"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="57">
+      <c r="G14" s="57"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="56">
         <f>Moorings!A15</f>
         <v>0</v>
       </c>
-      <c r="B15" s="57" t="str">
+      <c r="B15" s="56" t="str">
         <f>IF(D15="Mooring",Moorings!B15,"")</f>
         <v/>
       </c>
-      <c r="C15" s="58" t="str">
+      <c r="C15" s="57" t="str">
         <f>IF(D15="Sensor",Moorings!B15,"")</f>
         <v/>
       </c>
@@ -3864,22 +4135,22 @@
         <f>Moorings!C15</f>
         <v>0</v>
       </c>
-      <c r="F15" s="59" t="str">
+      <c r="F15" s="58" t="str">
         <f>IF(D15="Mooring",Moorings!E15,"")</f>
         <v/>
       </c>
-      <c r="G15" s="58"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="57">
+      <c r="G15" s="57"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="56">
         <f>Moorings!A16</f>
         <v>0</v>
       </c>
-      <c r="B16" s="57" t="str">
+      <c r="B16" s="56" t="str">
         <f>IF(D16="Mooring",Moorings!B16,"")</f>
         <v/>
       </c>
-      <c r="C16" s="58" t="str">
+      <c r="C16" s="57" t="str">
         <f>IF(D16="Sensor",Moorings!B16,"")</f>
         <v/>
       </c>
@@ -3891,11 +4162,11 @@
         <f>Moorings!C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="59" t="str">
+      <c r="F16" s="58" t="str">
         <f>IF(D16="Mooring",Moorings!E16,"")</f>
         <v/>
       </c>
-      <c r="G16" s="58"/>
+      <c r="G16" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3913,428 +4184,428 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="62" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="66"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1">
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="65"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="64"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1">
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="63"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="66"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1">
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="65"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="66"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1">
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="65"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="66"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1">
+      <c r="F6" s="63"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="65"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="66"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="66"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="B9" s="64"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="66"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="B10" s="64"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="66"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="B11" s="64"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="66"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="B12" s="64"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="64" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="65"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="65"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="65"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="65"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="63"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="65"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="B13" s="64"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="73" t="s">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="63"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="73" t="s">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="73" t="s">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="73" t="s">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1">
-      <c r="B17" s="64"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="73" t="s">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15" customHeight="1">
-      <c r="B18" s="64"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="73" t="s">
+    <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15" customHeight="1">
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="73" t="s">
+    <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="63"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15" customHeight="1">
-      <c r="B20" s="69" t="str">
+    <row r="20" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="68" t="str">
         <f>CONCATENATE(COUNTIF(B2:B19,"yes"),"/",COUNTA(B2:B19))</f>
         <v>6/6</v>
       </c>
-      <c r="C20" s="69" t="str">
+      <c r="C20" s="68" t="str">
         <f>CONCATENATE("'",COUNTIF(C2:C19,"yes"),"/",COUNTA(C2:C19))</f>
         <v>'0/6</v>
       </c>
-      <c r="D20" s="70" t="str">
+      <c r="D20" s="69" t="str">
         <f t="shared" ref="D20:E20" si="0">CONCATENATE("'",COUNTIF(D2:D19,"1/*")+COUNTIF(D2:D19,"2/*")*2,"/",COUNTIF(D2:D19,"*/1")+COUNTIF(D2:D19,"*/2")*2)</f>
         <v>'12/12</v>
       </c>
-      <c r="E20" s="70" t="str">
+      <c r="E20" s="69" t="str">
         <f t="shared" si="0"/>
         <v>'10/10</v>
       </c>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="73" t="s">
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15" customHeight="1">
-      <c r="B21" s="66"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="73" t="s">
+    <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="65"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15" customHeight="1">
-      <c r="B22" s="66"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="73" t="s">
+    <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="65"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15" customHeight="1">
-      <c r="B23" s="66"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="73" t="s">
+    <row r="23" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="65"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15" customHeight="1">
-      <c r="B24" s="66"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="73" t="s">
+    <row r="24" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="65"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15" customHeight="1">
-      <c r="B25" s="66"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="73" t="s">
+    <row r="25" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="65"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="72" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>